<commit_message>
Improved timetable reading and now it shows classes but still bugs
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/timetable.xlsx
+++ b/app/src/main/res/raw/timetable.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firzoknadeem/Documents/Android Studio Projects/SMD_Project/app/src/main/res/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{04F3E631-4B69-2A43-AA69-A6D977D3C018}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5235"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time Table" sheetId="13" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="340">
   <si>
     <t>Department of Computer Science</t>
   </si>
@@ -487,9 +493,6 @@
     <t>COAL LAB (B)</t>
   </si>
   <si>
-    <t>CP (A) 12:50 to 02:15</t>
-  </si>
-  <si>
     <t>CP Lab (A)</t>
   </si>
   <si>
@@ -520,12 +523,6 @@
     <t xml:space="preserve">Crypto graphy 01:00 to 02:25 </t>
   </si>
   <si>
-    <t xml:space="preserve">CP (B) 2:30  to 03:55        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cal-II (A) 11:30  to 12:50       </t>
-  </si>
-  <si>
     <t>Management (B ) 02:30 to 03:55            Management (C ) 04:00 to 05:25</t>
   </si>
   <si>
@@ -679,9 +676,6 @@
     <t>NLP10:30 to 11:50</t>
   </si>
   <si>
-    <t>NLP 10:30 to 11:50</t>
-  </si>
-  <si>
     <t>ACA 10:30 to 11:50</t>
   </si>
   <si>
@@ -910,9 +904,6 @@
     <t>Prob (A) 02:00 3:25                        Prob (B) 03:30 to 05:25</t>
   </si>
   <si>
-    <t>Adv. Prog. (C) 12:50 to 02:15</t>
-  </si>
-  <si>
     <t xml:space="preserve">                    Advance Prog Section D 02:00 to 04:50</t>
   </si>
   <si>
@@ -991,9 +982,6 @@
     <t>ML</t>
   </si>
   <si>
-    <t>RSC  Prob ( C) 12:02:15</t>
-  </si>
-  <si>
     <t>Time Table Ver-III A</t>
   </si>
   <si>
@@ -1003,18 +991,6 @@
     <t xml:space="preserve">DWH B 02:00 to 03:25                   </t>
   </si>
   <si>
-    <t>RSC History Secction D</t>
-  </si>
-  <si>
-    <t>RSC English (A)</t>
-  </si>
-  <si>
-    <t>RSC English (C)</t>
-  </si>
-  <si>
-    <t>RSC English (B)</t>
-  </si>
-  <si>
     <t>Stats &amp; Math (A1) 08:30 to 10:00</t>
   </si>
   <si>
@@ -1033,15 +1009,6 @@
     <t>Stats &amp; Math (A1) 12:00 to 01:25</t>
   </si>
   <si>
-    <t>RSC DS Section D</t>
-  </si>
-  <si>
-    <t>RSC DS Section E (04:00 to 04:55</t>
-  </si>
-  <si>
-    <t>RSC DS  Section F 03:00 to 03:55</t>
-  </si>
-  <si>
     <t>Professional Isues In IT 04:00 to 05:25</t>
   </si>
   <si>
@@ -1055,13 +1022,31 @@
   </si>
   <si>
     <t>PF Lab (D2) 11:30 to 03:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cal-II (A) </t>
+  </si>
+  <si>
+    <t>CP (A)</t>
+  </si>
+  <si>
+    <t>CP (B)</t>
+  </si>
+  <si>
+    <t>Adv. Prog. ©</t>
+  </si>
+  <si>
+    <t>Islamic (G)</t>
+  </si>
+  <si>
+    <t>NLP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="35">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3579,11 +3564,11 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="42" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="49" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="39" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3729,12 +3714,6 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3778,6 +3757,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="39" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="43" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3835,6 +3820,21 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="35" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3856,6 +3856,9 @@
     <xf numFmtId="0" fontId="20" fillId="42" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="42" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3964,9 +3967,6 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4063,25 +4063,7 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4114,6 +4096,15 @@
     <xf numFmtId="0" fontId="23" fillId="37" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="42" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4301,12 +4292,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="49" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4356,6 +4341,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -4402,7 +4395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4434,9 +4427,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4468,6 +4479,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4643,86 +4672,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ED165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:D19"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="17" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="17" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="25.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="92" width="9.140625" style="7"/>
-    <col min="93" max="134" width="9.140625" style="2"/>
-    <col min="135" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="5.6640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="25.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="92" width="9.1640625" style="7"/>
+    <col min="93" max="134" width="9.1640625" style="2"/>
+    <col min="135" max="16384" width="9.1640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="C1" s="434" t="s">
+    <row r="1" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="439" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="434"/>
-      <c r="E1" s="434"/>
+      <c r="D1" s="439"/>
+      <c r="E1" s="439"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="C2" s="435" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="435"/>
-      <c r="E2" s="435"/>
+    <row r="2" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="440" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="440"/>
+      <c r="E2" s="440"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="J2" s="496" t="s">
-        <v>326</v>
-      </c>
-      <c r="K2" s="497"/>
-      <c r="L2" s="498"/>
-    </row>
-    <row r="3" spans="1:134" ht="15" customHeight="1">
+      <c r="J2" s="498" t="s">
+        <v>320</v>
+      </c>
+      <c r="K2" s="499"/>
+      <c r="L2" s="500"/>
+    </row>
+    <row r="3" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="35"/>
       <c r="D3" s="35"/>
       <c r="E3" s="35"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="J3" s="125" t="s">
-        <v>226</v>
-      </c>
-      <c r="K3" s="509"/>
-      <c r="L3" s="510"/>
-    </row>
-    <row r="4" spans="1:134" ht="15" customHeight="1">
+        <v>222</v>
+      </c>
+      <c r="K3" s="511"/>
+      <c r="L3" s="512"/>
+    </row>
+    <row r="4" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F4" s="24"/>
       <c r="J4" s="183" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="L4" s="126" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:134" ht="15" customHeight="1" thickBot="1">
+    <row r="5" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="I5" s="6"/>
       <c r="J5" s="127" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="K5" s="128" t="s">
         <v>96</v>
@@ -4731,7 +4760,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:134" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
@@ -4765,8 +4794,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:134" ht="15" customHeight="1">
-      <c r="A7" s="346" t="s">
+    <row r="7" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="344" t="s">
         <v>94</v>
       </c>
       <c r="B7" s="109" t="s">
@@ -4781,16 +4810,16 @@
       <c r="E7" s="113" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="441" t="s">
+      <c r="F7" s="446" t="s">
         <v>50</v>
       </c>
       <c r="G7" s="161" t="s">
-        <v>169</v>
+        <v>334</v>
       </c>
       <c r="H7" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="I7" s="441" t="s">
+        <v>335</v>
+      </c>
+      <c r="I7" s="446" t="s">
         <v>48</v>
       </c>
       <c r="J7" s="255" t="s">
@@ -4799,10 +4828,10 @@
       <c r="K7" s="291"/>
       <c r="L7" s="292"/>
     </row>
-    <row r="8" spans="1:134" ht="15" customHeight="1">
-      <c r="A8" s="347"/>
+    <row r="8" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="345"/>
       <c r="B8" s="110" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C8" s="95"/>
       <c r="D8" s="40" t="s">
@@ -4811,24 +4840,24 @@
       <c r="E8" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="442"/>
+      <c r="F8" s="447"/>
       <c r="G8" s="158" t="s">
         <v>117</v>
       </c>
       <c r="H8" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="442"/>
-      <c r="J8" s="499" t="s">
-        <v>168</v>
-      </c>
-      <c r="K8" s="500"/>
+      <c r="I8" s="447"/>
+      <c r="J8" s="501" t="s">
+        <v>336</v>
+      </c>
+      <c r="K8" s="502"/>
       <c r="L8" s="260" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:134" ht="15" customHeight="1">
-      <c r="A9" s="347"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="345"/>
       <c r="B9" s="110" t="s">
         <v>47</v>
       </c>
@@ -4839,26 +4868,26 @@
         <v>103</v>
       </c>
       <c r="E9" s="117" t="s">
-        <v>218</v>
-      </c>
-      <c r="F9" s="442"/>
+        <v>215</v>
+      </c>
+      <c r="F9" s="447"/>
       <c r="G9" s="137" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="442"/>
+      <c r="I9" s="447"/>
       <c r="J9" s="176" t="s">
-        <v>203</v>
-      </c>
-      <c r="K9" s="294" t="s">
-        <v>342</v>
-      </c>
-      <c r="L9" s="295"/>
-    </row>
-    <row r="10" spans="1:134" ht="15" customHeight="1">
-      <c r="A10" s="347"/>
+        <v>200</v>
+      </c>
+      <c r="K9" s="359" t="s">
+        <v>329</v>
+      </c>
+      <c r="L9" s="360"/>
+    </row>
+    <row r="10" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="345"/>
       <c r="B10" s="110" t="s">
         <v>43</v>
       </c>
@@ -4871,22 +4900,22 @@
       <c r="E10" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="442"/>
+      <c r="F10" s="447"/>
       <c r="G10" s="158" t="s">
         <v>121</v>
       </c>
       <c r="H10" s="89" t="s">
-        <v>298</v>
-      </c>
-      <c r="I10" s="442"/>
-      <c r="J10" s="456" t="s">
-        <v>170</v>
-      </c>
-      <c r="K10" s="458"/>
-      <c r="L10" s="459"/>
-    </row>
-    <row r="11" spans="1:134" ht="15" customHeight="1">
-      <c r="A11" s="347"/>
+        <v>337</v>
+      </c>
+      <c r="I10" s="447"/>
+      <c r="J10" s="380" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" s="473"/>
+      <c r="L10" s="474"/>
+    </row>
+    <row r="11" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="345"/>
       <c r="B11" s="110" t="s">
         <v>41</v>
       </c>
@@ -4899,24 +4928,24 @@
       <c r="E11" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="F11" s="442"/>
+      <c r="F11" s="447"/>
       <c r="G11" s="159" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="I11" s="442"/>
+      <c r="I11" s="447"/>
       <c r="J11" s="206" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K11" s="40" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L11" s="42"/>
     </row>
-    <row r="12" spans="1:134" ht="15" customHeight="1">
-      <c r="A12" s="347"/>
+    <row r="12" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="345"/>
       <c r="B12" s="110" t="s">
         <v>38</v>
       </c>
@@ -4929,20 +4958,20 @@
       <c r="E12" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="442"/>
+      <c r="F12" s="447"/>
       <c r="G12" s="158" t="s">
         <v>129</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="I12" s="442"/>
+        <v>244</v>
+      </c>
+      <c r="I12" s="447"/>
       <c r="J12" s="256"/>
       <c r="K12" s="243"/>
       <c r="L12" s="221"/>
     </row>
-    <row r="13" spans="1:134" ht="15" customHeight="1">
-      <c r="A13" s="347"/>
+    <row r="13" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="345"/>
       <c r="B13" s="110" t="s">
         <v>35</v>
       </c>
@@ -4955,42 +4984,42 @@
       <c r="E13" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="442"/>
+      <c r="F13" s="447"/>
       <c r="G13" s="158" t="s">
         <v>133</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="442"/>
-      <c r="J13" s="463" t="s">
-        <v>197</v>
-      </c>
-      <c r="K13" s="464"/>
+      <c r="I13" s="447"/>
+      <c r="J13" s="462" t="s">
+        <v>194</v>
+      </c>
+      <c r="K13" s="463"/>
       <c r="L13" s="41"/>
     </row>
-    <row r="14" spans="1:134" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="347"/>
+    <row r="14" spans="1:134" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="345"/>
       <c r="B14" s="110" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C14" s="123"/>
       <c r="D14" s="40" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>228</v>
-      </c>
-      <c r="F14" s="442"/>
+        <v>224</v>
+      </c>
+      <c r="F14" s="447"/>
       <c r="G14" s="158" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="I14" s="442"/>
+        <v>338</v>
+      </c>
+      <c r="I14" s="447"/>
       <c r="J14" s="206" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="K14" s="220"/>
       <c r="L14" s="221"/>
@@ -5119,8 +5148,8 @@
       <c r="EC14" s="30"/>
       <c r="ED14" s="30"/>
     </row>
-    <row r="15" spans="1:134" ht="15" customHeight="1">
-      <c r="A15" s="347"/>
+    <row r="15" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="345"/>
       <c r="B15" s="110" t="s">
         <v>31</v>
       </c>
@@ -5131,24 +5160,24 @@
         <v>66</v>
       </c>
       <c r="E15" s="86" t="s">
-        <v>221</v>
-      </c>
-      <c r="F15" s="442"/>
+        <v>339</v>
+      </c>
+      <c r="F15" s="447"/>
       <c r="G15" s="137" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="442"/>
+      <c r="I15" s="447"/>
       <c r="J15" s="137" t="s">
         <v>73</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="41"/>
     </row>
-    <row r="16" spans="1:134" ht="15" customHeight="1">
-      <c r="A16" s="347"/>
+    <row r="16" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="345"/>
       <c r="B16" s="110" t="s">
         <v>29</v>
       </c>
@@ -5161,22 +5190,22 @@
       <c r="E16" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="F16" s="442"/>
+      <c r="F16" s="447"/>
       <c r="G16" s="137" t="s">
         <v>28</v>
       </c>
       <c r="H16" s="245" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="442"/>
+      <c r="I16" s="447"/>
       <c r="J16" s="241" t="s">
         <v>146</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="41"/>
     </row>
-    <row r="17" spans="1:134" ht="15" customHeight="1">
-      <c r="A17" s="347"/>
+    <row r="17" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="345"/>
       <c r="B17" s="110" t="s">
         <v>25</v>
       </c>
@@ -5189,22 +5218,20 @@
       <c r="E17" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="442"/>
+      <c r="F17" s="447"/>
       <c r="G17" s="279" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="284" t="s">
-        <v>331</v>
-      </c>
-      <c r="I17" s="442"/>
-      <c r="J17" s="507" t="s">
-        <v>276</v>
-      </c>
-      <c r="K17" s="508"/>
+      <c r="H17" s="284"/>
+      <c r="I17" s="447"/>
+      <c r="J17" s="509" t="s">
+        <v>272</v>
+      </c>
+      <c r="K17" s="510"/>
       <c r="L17" s="173"/>
     </row>
-    <row r="18" spans="1:134" ht="15" customHeight="1">
-      <c r="A18" s="347"/>
+    <row r="18" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="345"/>
       <c r="B18" s="110" t="s">
         <v>24</v>
       </c>
@@ -5215,50 +5242,50 @@
       <c r="E18" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="442"/>
+      <c r="F18" s="447"/>
       <c r="G18" s="199" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H18" s="252" t="s">
-        <v>315</v>
-      </c>
-      <c r="I18" s="442"/>
+        <v>310</v>
+      </c>
+      <c r="I18" s="447"/>
       <c r="J18" s="257" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="41"/>
     </row>
-    <row r="19" spans="1:134" ht="15" customHeight="1">
-      <c r="A19" s="347"/>
+    <row r="19" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="345"/>
       <c r="B19" s="111" t="s">
-        <v>241</v>
-      </c>
-      <c r="C19" s="344" t="s">
-        <v>333</v>
-      </c>
-      <c r="D19" s="345"/>
+        <v>237</v>
+      </c>
+      <c r="C19" s="472" t="s">
+        <v>323</v>
+      </c>
+      <c r="D19" s="392"/>
       <c r="E19" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="442"/>
+      <c r="F19" s="447"/>
       <c r="G19" s="244" t="s">
         <v>44</v>
       </c>
       <c r="H19" s="80" t="s">
         <v>145</v>
       </c>
-      <c r="I19" s="442"/>
-      <c r="J19" s="511" t="s">
-        <v>273</v>
-      </c>
-      <c r="K19" s="512"/>
+      <c r="I19" s="447"/>
+      <c r="J19" s="513" t="s">
+        <v>269</v>
+      </c>
+      <c r="K19" s="514"/>
       <c r="L19" s="41"/>
     </row>
-    <row r="20" spans="1:134" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="347"/>
+    <row r="20" spans="1:134" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="345"/>
       <c r="B20" s="111" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C20" s="102" t="s">
         <v>46</v>
@@ -5269,18 +5296,16 @@
       <c r="E20" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="442"/>
-      <c r="G20" s="253" t="s">
-        <v>330</v>
-      </c>
+      <c r="F20" s="447"/>
+      <c r="G20" s="253"/>
       <c r="H20" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="I20" s="442"/>
-      <c r="J20" s="517" t="s">
-        <v>303</v>
-      </c>
-      <c r="K20" s="518"/>
+        <v>166</v>
+      </c>
+      <c r="I20" s="447"/>
+      <c r="J20" s="519" t="s">
+        <v>298</v>
+      </c>
+      <c r="K20" s="520"/>
       <c r="L20" s="41"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -5405,29 +5430,27 @@
       <c r="EC20" s="7"/>
       <c r="ED20" s="7"/>
     </row>
-    <row r="21" spans="1:134" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A21" s="347"/>
+    <row r="21" spans="1:134" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="345"/>
       <c r="B21" s="112" t="s">
-        <v>243</v>
-      </c>
-      <c r="C21" s="352" t="s">
-        <v>184</v>
+        <v>239</v>
+      </c>
+      <c r="C21" s="350" t="s">
+        <v>181</v>
       </c>
       <c r="D21" s="369"/>
       <c r="E21" s="124" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="442"/>
+      <c r="F21" s="447"/>
       <c r="G21" s="39" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H21" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="I21" s="454"/>
-      <c r="J21" s="258" t="s">
-        <v>332</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="I21" s="459"/>
+      <c r="J21" s="258"/>
       <c r="K21" s="254"/>
       <c r="L21" s="103"/>
       <c r="M21" s="7"/>
@@ -5553,8 +5576,8 @@
       <c r="EC21" s="7"/>
       <c r="ED21" s="7"/>
     </row>
-    <row r="22" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A22" s="347"/>
+    <row r="22" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="345"/>
       <c r="B22" s="49" t="s">
         <v>19</v>
       </c>
@@ -5563,73 +5586,73 @@
       </c>
       <c r="D22" s="309"/>
       <c r="E22" s="310"/>
-      <c r="F22" s="442"/>
+      <c r="F22" s="447"/>
       <c r="G22" s="308" t="s">
         <v>65</v>
       </c>
       <c r="H22" s="309"/>
-      <c r="I22" s="445"/>
+      <c r="I22" s="450"/>
       <c r="J22" s="361" t="s">
         <v>15</v>
       </c>
       <c r="K22" s="309"/>
       <c r="L22" s="310"/>
     </row>
-    <row r="23" spans="1:134" ht="15" customHeight="1">
-      <c r="A23" s="347"/>
+    <row r="23" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="345"/>
       <c r="B23" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="448" t="s">
-        <v>188</v>
-      </c>
-      <c r="D23" s="449"/>
-      <c r="E23" s="450"/>
-      <c r="F23" s="443"/>
-      <c r="G23" s="448" t="s">
-        <v>189</v>
-      </c>
-      <c r="H23" s="449"/>
-      <c r="I23" s="450"/>
-      <c r="J23" s="357" t="s">
+      <c r="C23" s="453" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="454"/>
+      <c r="E23" s="455"/>
+      <c r="F23" s="448"/>
+      <c r="G23" s="453" t="s">
+        <v>186</v>
+      </c>
+      <c r="H23" s="454"/>
+      <c r="I23" s="455"/>
+      <c r="J23" s="355" t="s">
         <v>11</v>
       </c>
-      <c r="K23" s="358"/>
-      <c r="L23" s="359"/>
-    </row>
-    <row r="24" spans="1:134" ht="15" customHeight="1">
-      <c r="A24" s="347"/>
+      <c r="K23" s="356"/>
+      <c r="L23" s="357"/>
+    </row>
+    <row r="24" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="345"/>
       <c r="B24" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="455" t="s">
-        <v>259</v>
-      </c>
-      <c r="D24" s="456"/>
-      <c r="E24" s="457"/>
-      <c r="F24" s="443"/>
-      <c r="G24" s="465" t="s">
+      <c r="C24" s="460" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" s="380"/>
+      <c r="E24" s="461"/>
+      <c r="F24" s="448"/>
+      <c r="G24" s="464" t="s">
         <v>92</v>
       </c>
-      <c r="H24" s="466"/>
-      <c r="I24" s="467"/>
-      <c r="J24" s="470" t="s">
+      <c r="H24" s="465"/>
+      <c r="I24" s="466"/>
+      <c r="J24" s="469" t="s">
         <v>63</v>
       </c>
-      <c r="K24" s="471"/>
-      <c r="L24" s="472"/>
-    </row>
-    <row r="25" spans="1:134" ht="15" customHeight="1">
-      <c r="A25" s="347"/>
+      <c r="K24" s="470"/>
+      <c r="L24" s="471"/>
+    </row>
+    <row r="25" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="345"/>
       <c r="B25" s="105" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="247"/>
       <c r="D25" s="248"/>
       <c r="E25" s="252" t="s">
-        <v>334</v>
-      </c>
-      <c r="F25" s="443"/>
+        <v>324</v>
+      </c>
+      <c r="F25" s="448"/>
       <c r="G25" s="340"/>
       <c r="H25" s="341"/>
       <c r="I25" s="342"/>
@@ -5639,33 +5662,33 @@
       <c r="K25" s="312"/>
       <c r="L25" s="313"/>
     </row>
-    <row r="26" spans="1:134" ht="15" customHeight="1">
-      <c r="A26" s="347"/>
+    <row r="26" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="345"/>
       <c r="B26" s="105" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="370"/>
       <c r="D26" s="371"/>
       <c r="E26" s="372"/>
-      <c r="F26" s="443"/>
+      <c r="F26" s="448"/>
       <c r="G26" s="377"/>
       <c r="H26" s="377"/>
       <c r="I26" s="377"/>
-      <c r="J26" s="455" t="s">
-        <v>260</v>
-      </c>
-      <c r="K26" s="456"/>
+      <c r="J26" s="460" t="s">
+        <v>256</v>
+      </c>
+      <c r="K26" s="380"/>
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:134" ht="15" customHeight="1">
-      <c r="A27" s="347"/>
+    <row r="27" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="345"/>
       <c r="B27" s="105" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="370"/>
       <c r="D27" s="371"/>
       <c r="E27" s="372"/>
-      <c r="F27" s="443"/>
+      <c r="F27" s="448"/>
       <c r="G27" s="341"/>
       <c r="H27" s="341"/>
       <c r="I27" s="341"/>
@@ -5673,17 +5696,17 @@
       <c r="K27" s="335"/>
       <c r="L27" s="336"/>
     </row>
-    <row r="28" spans="1:134" ht="15" customHeight="1">
-      <c r="A28" s="347"/>
+    <row r="28" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="345"/>
       <c r="B28" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="479" t="s">
-        <v>229</v>
-      </c>
-      <c r="D28" s="480"/>
-      <c r="E28" s="481"/>
-      <c r="F28" s="443"/>
+      <c r="C28" s="481" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" s="482"/>
+      <c r="E28" s="483"/>
+      <c r="F28" s="448"/>
       <c r="G28" s="314"/>
       <c r="H28" s="314"/>
       <c r="I28" s="314"/>
@@ -5691,25 +5714,25 @@
       <c r="K28" s="335"/>
       <c r="L28" s="336"/>
     </row>
-    <row r="29" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A29" s="348"/>
+    <row r="29" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="346"/>
       <c r="B29" s="122" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="482" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29" s="436"/>
-      <c r="E29" s="437"/>
-      <c r="F29" s="444"/>
-      <c r="G29" s="438"/>
-      <c r="H29" s="439"/>
-      <c r="I29" s="440"/>
+        <v>159</v>
+      </c>
+      <c r="C29" s="484" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="441"/>
+      <c r="E29" s="442"/>
+      <c r="F29" s="449"/>
+      <c r="G29" s="443"/>
+      <c r="H29" s="444"/>
+      <c r="I29" s="445"/>
       <c r="J29" s="337"/>
       <c r="K29" s="338"/>
       <c r="L29" s="339"/>
     </row>
-    <row r="30" spans="1:134" ht="15" customHeight="1" thickBot="1">
+    <row r="30" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
@@ -5743,42 +5766,40 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:134" ht="15" customHeight="1">
-      <c r="A31" s="346" t="s">
+    <row r="31" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="344" t="s">
         <v>89</v>
       </c>
       <c r="B31" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="483" t="s">
-        <v>291</v>
-      </c>
-      <c r="D31" s="484"/>
+      <c r="C31" s="485" t="s">
+        <v>287</v>
+      </c>
+      <c r="D31" s="486"/>
       <c r="E31" s="116" t="s">
-        <v>335</v>
-      </c>
-      <c r="F31" s="451" t="s">
+        <v>325</v>
+      </c>
+      <c r="F31" s="456" t="s">
         <v>50</v>
       </c>
       <c r="G31" s="207" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="231" t="s">
-        <v>325</v>
-      </c>
-      <c r="I31" s="485" t="s">
+      <c r="H31" s="231"/>
+      <c r="I31" s="487" t="s">
         <v>48</v>
       </c>
       <c r="J31" s="275" t="s">
         <v>145</v>
       </c>
       <c r="K31" s="304" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="L31" s="305"/>
     </row>
-    <row r="32" spans="1:134" ht="15" customHeight="1">
-      <c r="A32" s="347"/>
+    <row r="32" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="345"/>
       <c r="B32" s="141" t="s">
         <v>47</v>
       </c>
@@ -5788,26 +5809,26 @@
       <c r="E32" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="F32" s="452"/>
+      <c r="F32" s="457"/>
       <c r="G32" s="201" t="s">
         <v>44</v>
       </c>
       <c r="H32" s="226" t="s">
-        <v>284</v>
-      </c>
-      <c r="I32" s="486"/>
+        <v>280</v>
+      </c>
+      <c r="I32" s="488"/>
       <c r="J32" s="175" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="K32" s="316" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="L32" s="330"/>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1">
-      <c r="A33" s="347"/>
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="345"/>
       <c r="B33" s="141" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C33" s="133" t="s">
         <v>46</v>
@@ -5818,27 +5839,27 @@
       <c r="E33" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="F33" s="452"/>
+      <c r="F33" s="457"/>
       <c r="G33" s="201" t="s">
         <v>104</v>
       </c>
       <c r="H33" s="66" t="s">
-        <v>244</v>
-      </c>
-      <c r="I33" s="486"/>
+        <v>240</v>
+      </c>
+      <c r="I33" s="488"/>
       <c r="J33" s="320" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K33" s="321"/>
       <c r="L33" s="42"/>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1">
-      <c r="A34" s="347"/>
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="345"/>
       <c r="B34" s="141" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="144" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D34" s="84" t="s">
         <v>142</v>
@@ -5846,20 +5867,20 @@
       <c r="E34" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="452"/>
+      <c r="F34" s="457"/>
       <c r="G34" s="204" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H34" s="51"/>
-      <c r="I34" s="486"/>
+      <c r="I34" s="488"/>
       <c r="J34" s="276" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K34" s="28"/>
       <c r="L34" s="42"/>
     </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1">
-      <c r="A35" s="347"/>
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="345"/>
       <c r="B35" s="141" t="s">
         <v>41</v>
       </c>
@@ -5870,24 +5891,24 @@
         <v>40</v>
       </c>
       <c r="E35" s="117" t="s">
-        <v>222</v>
-      </c>
-      <c r="F35" s="452"/>
+        <v>218</v>
+      </c>
+      <c r="F35" s="457"/>
       <c r="G35" s="203" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H35" s="227"/>
-      <c r="I35" s="486"/>
+      <c r="I35" s="488"/>
       <c r="J35" s="276" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="K35" s="28"/>
       <c r="L35" s="277" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1">
-      <c r="A36" s="347"/>
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="345"/>
       <c r="B36" s="141" t="s">
         <v>38</v>
       </c>
@@ -5898,24 +5919,24 @@
       <c r="E36" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="452"/>
+      <c r="F36" s="457"/>
       <c r="G36" s="204" t="s">
         <v>49</v>
       </c>
       <c r="H36" s="222" t="s">
         <v>146</v>
       </c>
-      <c r="I36" s="486"/>
+      <c r="I36" s="488"/>
       <c r="J36" s="280" t="s">
-        <v>208</v>
-      </c>
-      <c r="K36" s="490" t="s">
-        <v>319</v>
+        <v>205</v>
+      </c>
+      <c r="K36" s="492" t="s">
+        <v>314</v>
       </c>
       <c r="L36" s="343"/>
     </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1">
-      <c r="A37" s="347"/>
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="345"/>
       <c r="B37" s="141" t="s">
         <v>35</v>
       </c>
@@ -5928,22 +5949,22 @@
       <c r="E37" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="452"/>
+      <c r="F37" s="457"/>
       <c r="G37" s="98" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H37" s="228" t="s">
-        <v>313</v>
-      </c>
-      <c r="I37" s="486"/>
+        <v>308</v>
+      </c>
+      <c r="I37" s="488"/>
       <c r="J37" s="317" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="K37" s="318"/>
       <c r="L37" s="319"/>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1">
-      <c r="A38" s="347"/>
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="345"/>
       <c r="B38" s="141" t="s">
         <v>33</v>
       </c>
@@ -5956,72 +5977,70 @@
       <c r="E38" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="452"/>
+      <c r="F38" s="457"/>
       <c r="G38" s="193" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H38" s="219" t="s">
-        <v>166</v>
-      </c>
-      <c r="I38" s="486"/>
-      <c r="J38" s="65" t="s">
-        <v>329</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="I38" s="488"/>
+      <c r="J38" s="65"/>
       <c r="K38" s="285"/>
       <c r="L38" s="286"/>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1">
-      <c r="A39" s="347"/>
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="345"/>
       <c r="B39" s="141" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="148" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="118" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="452"/>
+        <v>214</v>
+      </c>
+      <c r="F39" s="457"/>
       <c r="G39" s="201" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H39" s="219" t="s">
-        <v>195</v>
-      </c>
-      <c r="I39" s="486"/>
+        <v>192</v>
+      </c>
+      <c r="I39" s="488"/>
       <c r="J39" s="367" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="K39" s="368"/>
       <c r="L39" s="44"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1">
-      <c r="A40" s="347"/>
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="345"/>
       <c r="B40" s="141" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="145" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="63" t="s">
-        <v>312</v>
-      </c>
-      <c r="F40" s="452"/>
+        <v>307</v>
+      </c>
+      <c r="F40" s="457"/>
       <c r="G40" s="197" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H40" s="229"/>
-      <c r="I40" s="486"/>
-      <c r="J40" s="360" t="s">
+      <c r="I40" s="488"/>
+      <c r="J40" s="358" t="s">
         <v>81</v>
       </c>
-      <c r="K40" s="294"/>
-      <c r="L40" s="295"/>
-    </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1">
-      <c r="A41" s="347"/>
+      <c r="K40" s="359"/>
+      <c r="L40" s="360"/>
+    </row>
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="345"/>
       <c r="B41" s="141" t="s">
         <v>25</v>
       </c>
@@ -6034,22 +6053,22 @@
       <c r="E41" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="452"/>
+      <c r="F41" s="457"/>
       <c r="G41" s="193" t="s">
         <v>150</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="I41" s="486"/>
+        <v>210</v>
+      </c>
+      <c r="I41" s="488"/>
       <c r="J41" s="315" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K41" s="316"/>
       <c r="L41" s="42"/>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1">
-      <c r="A42" s="347"/>
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="345"/>
       <c r="B42" s="141" t="s">
         <v>24</v>
       </c>
@@ -6060,48 +6079,48 @@
         <v>154</v>
       </c>
       <c r="E42" s="119" t="s">
-        <v>283</v>
-      </c>
-      <c r="F42" s="452"/>
+        <v>279</v>
+      </c>
+      <c r="F42" s="457"/>
       <c r="G42" s="181" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H42" s="229"/>
-      <c r="I42" s="486"/>
-      <c r="J42" s="504" t="s">
-        <v>253</v>
-      </c>
-      <c r="K42" s="505"/>
-      <c r="L42" s="506"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1">
-      <c r="A43" s="347"/>
+      <c r="I42" s="488"/>
+      <c r="J42" s="506" t="s">
+        <v>249</v>
+      </c>
+      <c r="K42" s="507"/>
+      <c r="L42" s="508"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="345"/>
       <c r="B43" s="142" t="s">
-        <v>241</v>
-      </c>
-      <c r="C43" s="386" t="s">
-        <v>317</v>
-      </c>
-      <c r="D43" s="345"/>
+        <v>237</v>
+      </c>
+      <c r="C43" s="391" t="s">
+        <v>312</v>
+      </c>
+      <c r="D43" s="392"/>
       <c r="E43" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="452"/>
-      <c r="G43" s="468" t="s">
-        <v>295</v>
-      </c>
-      <c r="H43" s="469"/>
-      <c r="I43" s="486"/>
-      <c r="J43" s="360" t="s">
-        <v>276</v>
-      </c>
-      <c r="K43" s="294"/>
+      <c r="F43" s="457"/>
+      <c r="G43" s="467" t="s">
+        <v>291</v>
+      </c>
+      <c r="H43" s="468"/>
+      <c r="I43" s="488"/>
+      <c r="J43" s="358" t="s">
+        <v>272</v>
+      </c>
+      <c r="K43" s="359"/>
       <c r="L43" s="43"/>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1">
-      <c r="A44" s="347"/>
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="345"/>
       <c r="B44" s="142" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C44" s="138"/>
       <c r="D44" s="168" t="s">
@@ -6110,36 +6129,36 @@
       <c r="E44" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="F44" s="452"/>
+      <c r="F44" s="457"/>
       <c r="G44" s="95"/>
       <c r="H44" s="51"/>
-      <c r="I44" s="486"/>
+      <c r="I44" s="488"/>
       <c r="J44" s="325" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="K44" s="326"/>
       <c r="L44" s="327"/>
     </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" thickBot="1">
-      <c r="A45" s="347"/>
+    <row r="45" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="345"/>
       <c r="B45" s="143" t="s">
-        <v>243</v>
-      </c>
-      <c r="C45" s="488" t="s">
         <v>239</v>
       </c>
-      <c r="D45" s="488"/>
-      <c r="E45" s="489"/>
-      <c r="F45" s="452"/>
+      <c r="C45" s="490" t="s">
+        <v>235</v>
+      </c>
+      <c r="D45" s="490"/>
+      <c r="E45" s="491"/>
+      <c r="F45" s="457"/>
       <c r="G45" s="211"/>
       <c r="H45" s="230"/>
-      <c r="I45" s="487"/>
+      <c r="I45" s="489"/>
       <c r="J45" s="328"/>
       <c r="K45" s="329"/>
       <c r="L45" s="57"/>
     </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" thickBot="1">
-      <c r="A46" s="347"/>
+    <row r="46" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="345"/>
       <c r="B46" s="150" t="s">
         <v>19</v>
       </c>
@@ -6148,51 +6167,51 @@
       </c>
       <c r="D46" s="106"/>
       <c r="E46" s="120"/>
-      <c r="F46" s="442"/>
+      <c r="F46" s="447"/>
       <c r="G46" s="331" t="s">
         <v>65</v>
       </c>
       <c r="H46" s="332"/>
-      <c r="I46" s="445"/>
+      <c r="I46" s="450"/>
       <c r="J46" s="331" t="s">
         <v>15</v>
       </c>
       <c r="K46" s="332"/>
       <c r="L46" s="333"/>
     </row>
-    <row r="47" spans="1:12" ht="15" customHeight="1">
-      <c r="A47" s="347"/>
+    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="345"/>
       <c r="B47" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="473" t="s">
+      <c r="C47" s="475" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="474"/>
-      <c r="E47" s="475"/>
-      <c r="F47" s="442"/>
-      <c r="G47" s="476" t="s">
+      <c r="D47" s="476"/>
+      <c r="E47" s="477"/>
+      <c r="F47" s="447"/>
+      <c r="G47" s="478" t="s">
         <v>107</v>
       </c>
-      <c r="H47" s="477"/>
-      <c r="I47" s="478"/>
-      <c r="J47" s="391" t="s">
+      <c r="H47" s="479"/>
+      <c r="I47" s="480"/>
+      <c r="J47" s="397" t="s">
         <v>86</v>
       </c>
-      <c r="K47" s="392"/>
-      <c r="L47" s="393"/>
-    </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1">
-      <c r="A48" s="347"/>
+      <c r="K47" s="398"/>
+      <c r="L47" s="399"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="345"/>
       <c r="B48" s="152" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="390" t="s">
+      <c r="C48" s="396" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="323"/>
       <c r="E48" s="324"/>
-      <c r="F48" s="442"/>
+      <c r="F48" s="447"/>
       <c r="G48" s="307" t="s">
         <v>108</v>
       </c>
@@ -6204,135 +6223,135 @@
       <c r="K48" s="323"/>
       <c r="L48" s="324"/>
     </row>
-    <row r="49" spans="1:134" ht="15" customHeight="1">
-      <c r="A49" s="347"/>
+    <row r="49" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="345"/>
       <c r="B49" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="390" t="s">
-        <v>171</v>
+      <c r="C49" s="396" t="s">
+        <v>168</v>
       </c>
       <c r="D49" s="323"/>
       <c r="E49" s="324"/>
-      <c r="F49" s="442"/>
+      <c r="F49" s="447"/>
       <c r="G49" s="307" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H49" s="307"/>
       <c r="I49" s="343"/>
       <c r="J49" s="322" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K49" s="323"/>
       <c r="L49" s="324"/>
     </row>
-    <row r="50" spans="1:134" ht="15" customHeight="1">
-      <c r="A50" s="347"/>
+    <row r="50" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="345"/>
       <c r="B50" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="390" t="s">
-        <v>172</v>
+      <c r="C50" s="396" t="s">
+        <v>169</v>
       </c>
       <c r="D50" s="323"/>
       <c r="E50" s="324"/>
-      <c r="F50" s="442"/>
+      <c r="F50" s="447"/>
       <c r="G50" s="340"/>
       <c r="H50" s="341"/>
       <c r="I50" s="342"/>
       <c r="J50" s="322" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K50" s="323"/>
       <c r="L50" s="324"/>
     </row>
-    <row r="51" spans="1:134" ht="15" customHeight="1">
-      <c r="A51" s="347"/>
+    <row r="51" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="345"/>
       <c r="B51" s="153" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="390" t="s">
-        <v>173</v>
+      <c r="C51" s="396" t="s">
+        <v>170</v>
       </c>
       <c r="D51" s="323"/>
       <c r="E51" s="324"/>
-      <c r="F51" s="442"/>
+      <c r="F51" s="447"/>
       <c r="G51" s="307" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H51" s="307"/>
       <c r="I51" s="343"/>
       <c r="J51" s="322" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K51" s="323"/>
       <c r="L51" s="324"/>
     </row>
-    <row r="52" spans="1:134" ht="15" customHeight="1">
-      <c r="A52" s="347"/>
+    <row r="52" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="345"/>
       <c r="B52" s="153" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="390" t="s">
-        <v>174</v>
+      <c r="C52" s="396" t="s">
+        <v>171</v>
       </c>
       <c r="D52" s="323"/>
       <c r="E52" s="324"/>
-      <c r="F52" s="442"/>
-      <c r="G52" s="397" t="s">
+      <c r="F52" s="447"/>
+      <c r="G52" s="403" t="s">
         <v>106</v>
       </c>
-      <c r="H52" s="397"/>
-      <c r="I52" s="398"/>
+      <c r="H52" s="403"/>
+      <c r="I52" s="404"/>
       <c r="J52" s="322" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K52" s="323"/>
       <c r="L52" s="324"/>
     </row>
-    <row r="53" spans="1:134" ht="15" customHeight="1">
-      <c r="A53" s="347"/>
+    <row r="53" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="345"/>
       <c r="B53" s="153" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="522" t="s">
+      <c r="C53" s="524" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="395"/>
-      <c r="E53" s="396"/>
-      <c r="F53" s="442"/>
+      <c r="D53" s="401"/>
+      <c r="E53" s="402"/>
+      <c r="F53" s="447"/>
       <c r="G53" s="340"/>
       <c r="H53" s="341"/>
       <c r="I53" s="342"/>
-      <c r="J53" s="394" t="s">
+      <c r="J53" s="400" t="s">
         <v>137</v>
       </c>
-      <c r="K53" s="395"/>
-      <c r="L53" s="396"/>
-    </row>
-    <row r="54" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A54" s="348"/>
+      <c r="K53" s="401"/>
+      <c r="L53" s="402"/>
+    </row>
+    <row r="54" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="346"/>
       <c r="B54" s="208" t="s">
-        <v>271</v>
-      </c>
-      <c r="C54" s="383" t="s">
-        <v>272</v>
-      </c>
-      <c r="D54" s="384"/>
-      <c r="E54" s="385"/>
-      <c r="F54" s="454"/>
-      <c r="G54" s="383" t="s">
-        <v>272</v>
-      </c>
-      <c r="H54" s="384"/>
-      <c r="I54" s="385"/>
-      <c r="J54" s="516" t="s">
+        <v>267</v>
+      </c>
+      <c r="C54" s="388" t="s">
+        <v>268</v>
+      </c>
+      <c r="D54" s="389"/>
+      <c r="E54" s="390"/>
+      <c r="F54" s="459"/>
+      <c r="G54" s="388" t="s">
+        <v>268</v>
+      </c>
+      <c r="H54" s="389"/>
+      <c r="I54" s="390"/>
+      <c r="J54" s="518" t="s">
         <v>3</v>
       </c>
-      <c r="K54" s="424"/>
-      <c r="L54" s="425"/>
-    </row>
-    <row r="55" spans="1:134" ht="15" customHeight="1" thickBot="1">
+      <c r="K54" s="429"/>
+      <c r="L54" s="430"/>
+    </row>
+    <row r="55" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
@@ -6366,8 +6385,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:134" ht="15" customHeight="1">
-      <c r="A56" s="346" t="s">
+    <row r="56" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="344" t="s">
         <v>82</v>
       </c>
       <c r="B56" s="140" t="s">
@@ -6382,7 +6401,7 @@
       <c r="E56" s="113" t="s">
         <v>101</v>
       </c>
-      <c r="F56" s="441" t="s">
+      <c r="F56" s="446" t="s">
         <v>50</v>
       </c>
       <c r="G56" s="108" t="s">
@@ -6391,19 +6410,19 @@
       <c r="H56" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="I56" s="451" t="s">
+      <c r="I56" s="456" t="s">
         <v>48</v>
       </c>
-      <c r="J56" s="527" t="s">
-        <v>232</v>
-      </c>
-      <c r="K56" s="528"/>
+      <c r="J56" s="529" t="s">
+        <v>228</v>
+      </c>
+      <c r="K56" s="530"/>
       <c r="L56" s="185" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:134" ht="15" customHeight="1">
-      <c r="A57" s="347"/>
+    <row r="57" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="345"/>
       <c r="B57" s="141" t="s">
         <v>33</v>
       </c>
@@ -6414,22 +6433,22 @@
       <c r="E57" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="F57" s="442"/>
+      <c r="F57" s="447"/>
       <c r="G57" s="65" t="s">
         <v>116</v>
       </c>
       <c r="H57" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="I57" s="452"/>
+      <c r="I57" s="457"/>
       <c r="J57" s="266" t="s">
         <v>117</v>
       </c>
       <c r="K57" s="188"/>
       <c r="L57" s="189"/>
     </row>
-    <row r="58" spans="1:134" ht="15" customHeight="1">
-      <c r="A58" s="347"/>
+    <row r="58" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="345"/>
       <c r="B58" s="141" t="s">
         <v>47</v>
       </c>
@@ -6440,26 +6459,26 @@
         <v>103</v>
       </c>
       <c r="E58" s="282" t="s">
-        <v>321</v>
-      </c>
-      <c r="F58" s="442"/>
+        <v>316</v>
+      </c>
+      <c r="F58" s="447"/>
       <c r="G58" s="56" t="s">
         <v>69</v>
       </c>
       <c r="H58" s="212" t="s">
-        <v>304</v>
-      </c>
-      <c r="I58" s="452"/>
+        <v>299</v>
+      </c>
+      <c r="I58" s="457"/>
       <c r="J58" s="92" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K58" s="262" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="L58" s="261"/>
     </row>
-    <row r="59" spans="1:134" ht="15" customHeight="1">
-      <c r="A59" s="347"/>
+    <row r="59" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="345"/>
       <c r="B59" s="141" t="s">
         <v>43</v>
       </c>
@@ -6472,27 +6491,27 @@
       <c r="E59" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="F59" s="442"/>
+      <c r="F59" s="447"/>
       <c r="G59" s="65" t="s">
         <v>121</v>
       </c>
       <c r="H59" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="I59" s="452"/>
+      <c r="I59" s="457"/>
       <c r="J59" s="183" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K59" s="2"/>
       <c r="L59" s="44"/>
     </row>
-    <row r="60" spans="1:134" ht="15" customHeight="1">
-      <c r="A60" s="347"/>
+    <row r="60" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="345"/>
       <c r="B60" s="141" t="s">
         <v>41</v>
       </c>
       <c r="C60" s="148" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D60" s="40" t="s">
         <v>123</v>
@@ -6500,24 +6519,24 @@
       <c r="E60" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="F60" s="442"/>
+      <c r="F60" s="447"/>
       <c r="G60" s="65" t="s">
         <v>125</v>
       </c>
       <c r="H60" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="I60" s="452"/>
+      <c r="I60" s="457"/>
       <c r="J60" s="266" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K60" s="267" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="L60" s="221"/>
     </row>
-    <row r="61" spans="1:134" ht="15" customHeight="1">
-      <c r="A61" s="347"/>
+    <row r="61" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="345"/>
       <c r="B61" s="141" t="s">
         <v>38</v>
       </c>
@@ -6530,20 +6549,20 @@
       <c r="E61" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F61" s="442"/>
+      <c r="F61" s="447"/>
       <c r="G61" s="65" t="s">
         <v>129</v>
       </c>
       <c r="H61" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="I61" s="452"/>
+        <v>244</v>
+      </c>
+      <c r="I61" s="457"/>
       <c r="J61" s="236"/>
       <c r="K61" s="11"/>
       <c r="L61" s="41"/>
     </row>
-    <row r="62" spans="1:134" ht="15" customHeight="1">
-      <c r="A62" s="347"/>
+    <row r="62" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="345"/>
       <c r="B62" s="141" t="s">
         <v>35</v>
       </c>
@@ -6556,42 +6575,42 @@
       <c r="E62" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="F62" s="442"/>
+      <c r="F62" s="447"/>
       <c r="G62" s="65" t="s">
         <v>133</v>
       </c>
       <c r="H62" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="I62" s="452"/>
-      <c r="J62" s="360" t="s">
-        <v>193</v>
-      </c>
-      <c r="K62" s="401"/>
+      <c r="I62" s="457"/>
+      <c r="J62" s="358" t="s">
+        <v>190</v>
+      </c>
+      <c r="K62" s="407"/>
       <c r="L62" s="192"/>
     </row>
-    <row r="63" spans="1:134" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="A63" s="347"/>
+    <row r="63" spans="1:134" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="345"/>
       <c r="B63" s="141" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C63" s="154"/>
       <c r="D63" s="40" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E63" s="54" t="s">
-        <v>228</v>
-      </c>
-      <c r="F63" s="442"/>
+        <v>224</v>
+      </c>
+      <c r="F63" s="447"/>
       <c r="G63" s="75" t="s">
         <v>71</v>
       </c>
       <c r="H63" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="I63" s="452"/>
+        <v>229</v>
+      </c>
+      <c r="I63" s="457"/>
       <c r="J63" s="317" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="K63" s="318"/>
       <c r="L63" s="319"/>
@@ -6718,8 +6737,8 @@
       <c r="EC63" s="31"/>
       <c r="ED63" s="31"/>
     </row>
-    <row r="64" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A64" s="347"/>
+    <row r="64" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="345"/>
       <c r="B64" s="141" t="s">
         <v>31</v>
       </c>
@@ -6730,21 +6749,21 @@
         <v>66</v>
       </c>
       <c r="E64" s="86" t="s">
-        <v>220</v>
-      </c>
-      <c r="F64" s="442"/>
+        <v>217</v>
+      </c>
+      <c r="F64" s="447"/>
       <c r="G64" s="75" t="s">
         <v>23</v>
       </c>
       <c r="H64" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="I64" s="452"/>
+      <c r="I64" s="457"/>
       <c r="J64" s="264" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K64" s="296" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="L64" s="297"/>
       <c r="M64" s="7"/>
@@ -6870,8 +6889,8 @@
       <c r="EC64" s="8"/>
       <c r="ED64" s="8"/>
     </row>
-    <row r="65" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A65" s="347"/>
+    <row r="65" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="345"/>
       <c r="B65" s="141" t="s">
         <v>29</v>
       </c>
@@ -6882,14 +6901,14 @@
       <c r="E65" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="F65" s="442"/>
+      <c r="F65" s="447"/>
       <c r="G65" s="85" t="s">
         <v>42</v>
       </c>
       <c r="H65" s="119" t="s">
-        <v>214</v>
-      </c>
-      <c r="I65" s="452"/>
+        <v>211</v>
+      </c>
+      <c r="I65" s="457"/>
       <c r="J65" s="265" t="s">
         <v>73</v>
       </c>
@@ -7018,8 +7037,8 @@
       <c r="EC65" s="8"/>
       <c r="ED65" s="8"/>
     </row>
-    <row r="66" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A66" s="347"/>
+    <row r="66" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="345"/>
       <c r="B66" s="141" t="s">
         <v>25</v>
       </c>
@@ -7032,16 +7051,16 @@
       <c r="E66" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="F66" s="442"/>
+      <c r="F66" s="447"/>
       <c r="G66" s="93" t="s">
         <v>70</v>
       </c>
       <c r="H66" s="79" t="s">
-        <v>209</v>
-      </c>
-      <c r="I66" s="452"/>
+        <v>206</v>
+      </c>
+      <c r="I66" s="457"/>
       <c r="J66" s="186" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K66" s="172"/>
       <c r="L66" s="173"/>
@@ -7168,8 +7187,8 @@
       <c r="EC66" s="8"/>
       <c r="ED66" s="8"/>
     </row>
-    <row r="67" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A67" s="347"/>
+    <row r="67" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="345"/>
       <c r="B67" s="141" t="s">
         <v>24</v>
       </c>
@@ -7182,12 +7201,12 @@
       <c r="E67" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="F67" s="442"/>
+      <c r="F67" s="447"/>
       <c r="G67" s="301" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="H67" s="302"/>
-      <c r="I67" s="452"/>
+      <c r="I67" s="457"/>
       <c r="J67" s="271"/>
       <c r="K67" s="270"/>
       <c r="L67" s="272"/>
@@ -7314,10 +7333,10 @@
       <c r="EC67" s="8"/>
       <c r="ED67" s="8"/>
     </row>
-    <row r="68" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A68" s="347"/>
+    <row r="68" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="345"/>
       <c r="B68" s="142" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C68" s="137" t="s">
         <v>64</v>
@@ -7326,18 +7345,18 @@
         <v>142</v>
       </c>
       <c r="E68" s="114" t="s">
-        <v>196</v>
-      </c>
-      <c r="F68" s="442"/>
+        <v>193</v>
+      </c>
+      <c r="F68" s="447"/>
       <c r="G68" s="75" t="s">
         <v>28</v>
       </c>
       <c r="H68" s="240" t="s">
-        <v>327</v>
-      </c>
-      <c r="I68" s="452"/>
+        <v>321</v>
+      </c>
+      <c r="I68" s="457"/>
       <c r="J68" s="317" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K68" s="318"/>
       <c r="L68" s="319"/>
@@ -7464,13 +7483,13 @@
       <c r="EC68" s="8"/>
       <c r="ED68" s="8"/>
     </row>
-    <row r="69" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A69" s="347"/>
+    <row r="69" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="345"/>
       <c r="B69" s="142" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C69" s="144" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D69" s="38" t="s">
         <v>87</v>
@@ -7478,16 +7497,16 @@
       <c r="E69" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="F69" s="442"/>
+      <c r="F69" s="447"/>
       <c r="G69" s="102" t="s">
         <v>49</v>
       </c>
       <c r="H69" s="78" t="s">
-        <v>198</v>
-      </c>
-      <c r="I69" s="452"/>
+        <v>195</v>
+      </c>
+      <c r="I69" s="457"/>
       <c r="J69" s="187" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K69" s="27"/>
       <c r="L69" s="46"/>
@@ -7614,26 +7633,26 @@
       <c r="EC69" s="8"/>
       <c r="ED69" s="8"/>
     </row>
-    <row r="70" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A70" s="347"/>
+    <row r="70" spans="1:134" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="345"/>
       <c r="B70" s="143" t="s">
-        <v>243</v>
-      </c>
-      <c r="C70" s="353" t="s">
-        <v>184</v>
+        <v>239</v>
+      </c>
+      <c r="C70" s="351" t="s">
+        <v>181</v>
       </c>
       <c r="D70" s="369"/>
       <c r="E70" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="F70" s="442"/>
+      <c r="F70" s="447"/>
       <c r="G70" s="88" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H70" s="67" t="s">
-        <v>187</v>
-      </c>
-      <c r="I70" s="453"/>
+        <v>184</v>
+      </c>
+      <c r="I70" s="458"/>
       <c r="J70" s="223"/>
       <c r="K70" s="224"/>
       <c r="L70" s="100"/>
@@ -7760,8 +7779,8 @@
       <c r="EC70" s="8"/>
       <c r="ED70" s="8"/>
     </row>
-    <row r="71" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A71" s="347"/>
+    <row r="71" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="345"/>
       <c r="B71" s="150" t="s">
         <v>19</v>
       </c>
@@ -7770,7 +7789,7 @@
       </c>
       <c r="D71" s="309"/>
       <c r="E71" s="310"/>
-      <c r="F71" s="442"/>
+      <c r="F71" s="447"/>
       <c r="G71" s="361" t="s">
         <v>65</v>
       </c>
@@ -7782,152 +7801,152 @@
       <c r="K71" s="332"/>
       <c r="L71" s="333"/>
     </row>
-    <row r="72" spans="1:134" ht="15" customHeight="1">
-      <c r="A72" s="347"/>
+    <row r="72" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="345"/>
       <c r="B72" s="232" t="s">
         <v>14</v>
       </c>
-      <c r="C72" s="523" t="s">
+      <c r="C72" s="525" t="s">
         <v>80</v>
       </c>
-      <c r="D72" s="458"/>
-      <c r="E72" s="524"/>
-      <c r="F72" s="442"/>
+      <c r="D72" s="473"/>
+      <c r="E72" s="526"/>
+      <c r="F72" s="447"/>
       <c r="G72" s="315" t="s">
         <v>156</v>
       </c>
       <c r="H72" s="316"/>
       <c r="I72" s="330"/>
       <c r="J72" s="198" t="s">
-        <v>301</v>
-      </c>
-      <c r="K72" s="399" t="s">
-        <v>302</v>
-      </c>
-      <c r="L72" s="400"/>
-    </row>
-    <row r="73" spans="1:134" ht="15" customHeight="1">
-      <c r="A73" s="347"/>
+        <v>296</v>
+      </c>
+      <c r="K72" s="405" t="s">
+        <v>297</v>
+      </c>
+      <c r="L72" s="406"/>
+    </row>
+    <row r="73" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="345"/>
       <c r="B73" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="456" t="s">
-        <v>257</v>
-      </c>
-      <c r="D73" s="456"/>
-      <c r="E73" s="423"/>
-      <c r="F73" s="442"/>
-      <c r="G73" s="460" t="s">
+      <c r="C73" s="380" t="s">
+        <v>253</v>
+      </c>
+      <c r="D73" s="380"/>
+      <c r="E73" s="381"/>
+      <c r="F73" s="447"/>
+      <c r="G73" s="382" t="s">
         <v>85</v>
       </c>
-      <c r="H73" s="461"/>
-      <c r="I73" s="462"/>
+      <c r="H73" s="383"/>
+      <c r="I73" s="384"/>
       <c r="J73" s="315" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="K73" s="316"/>
       <c r="L73" s="45"/>
       <c r="M73" s="16"/>
     </row>
-    <row r="74" spans="1:134" ht="15" customHeight="1">
-      <c r="A74" s="347"/>
+    <row r="74" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="345"/>
       <c r="B74" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="353" t="s">
-        <v>182</v>
-      </c>
-      <c r="D74" s="353"/>
+      <c r="C74" s="351" t="s">
+        <v>179</v>
+      </c>
+      <c r="D74" s="351"/>
       <c r="E74" s="297"/>
-      <c r="F74" s="442"/>
-      <c r="G74" s="352" t="s">
-        <v>183</v>
-      </c>
-      <c r="H74" s="353"/>
+      <c r="F74" s="447"/>
+      <c r="G74" s="350" t="s">
+        <v>180</v>
+      </c>
+      <c r="H74" s="351"/>
       <c r="I74" s="297"/>
-      <c r="J74" s="525"/>
+      <c r="J74" s="527"/>
       <c r="K74" s="314"/>
-      <c r="L74" s="526"/>
-    </row>
-    <row r="75" spans="1:134" ht="15" customHeight="1">
-      <c r="A75" s="347"/>
+      <c r="L74" s="528"/>
+    </row>
+    <row r="75" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="345"/>
       <c r="B75" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="353" t="s">
-        <v>190</v>
-      </c>
-      <c r="D75" s="353"/>
+      <c r="C75" s="351" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="351"/>
       <c r="E75" s="297"/>
-      <c r="F75" s="442"/>
+      <c r="F75" s="447"/>
       <c r="G75" s="340"/>
       <c r="H75" s="341"/>
       <c r="I75" s="342"/>
       <c r="J75" s="306" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K75" s="307"/>
       <c r="L75" s="343"/>
     </row>
-    <row r="76" spans="1:134" ht="15" customHeight="1">
-      <c r="A76" s="347"/>
+    <row r="76" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="345"/>
       <c r="B76" s="141" t="s">
         <v>6</v>
       </c>
       <c r="C76" s="341"/>
       <c r="D76" s="341"/>
       <c r="E76" s="342"/>
-      <c r="F76" s="442"/>
-      <c r="G76" s="525"/>
+      <c r="F76" s="447"/>
+      <c r="G76" s="527"/>
       <c r="H76" s="314"/>
-      <c r="I76" s="526"/>
+      <c r="I76" s="528"/>
       <c r="J76" s="306" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K76" s="307"/>
       <c r="L76" s="343"/>
     </row>
-    <row r="77" spans="1:134" ht="15" customHeight="1">
-      <c r="A77" s="347"/>
+    <row r="77" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="345"/>
       <c r="B77" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="446" t="s">
-        <v>229</v>
-      </c>
-      <c r="D77" s="446"/>
-      <c r="E77" s="447"/>
-      <c r="F77" s="442"/>
-      <c r="G77" s="521" t="s">
-        <v>229</v>
-      </c>
-      <c r="H77" s="446"/>
-      <c r="I77" s="447"/>
-      <c r="J77" s="521" t="s">
-        <v>229</v>
-      </c>
-      <c r="K77" s="446"/>
-      <c r="L77" s="447"/>
-    </row>
-    <row r="78" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A78" s="348"/>
+      <c r="C77" s="451" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="451"/>
+      <c r="E77" s="452"/>
+      <c r="F77" s="447"/>
+      <c r="G77" s="523" t="s">
+        <v>225</v>
+      </c>
+      <c r="H77" s="451"/>
+      <c r="I77" s="452"/>
+      <c r="J77" s="523" t="s">
+        <v>225</v>
+      </c>
+      <c r="K77" s="451"/>
+      <c r="L77" s="452"/>
+    </row>
+    <row r="78" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="346"/>
       <c r="B78" s="233" t="s">
+        <v>159</v>
+      </c>
+      <c r="C78" s="441" t="s">
         <v>160</v>
       </c>
-      <c r="C78" s="436" t="s">
-        <v>161</v>
-      </c>
-      <c r="D78" s="436"/>
-      <c r="E78" s="437"/>
-      <c r="F78" s="454"/>
-      <c r="G78" s="409"/>
-      <c r="H78" s="410"/>
-      <c r="I78" s="411"/>
-      <c r="J78" s="513"/>
-      <c r="K78" s="514"/>
-      <c r="L78" s="515"/>
-    </row>
-    <row r="79" spans="1:134" ht="15" customHeight="1" thickBot="1">
+      <c r="D78" s="441"/>
+      <c r="E78" s="442"/>
+      <c r="F78" s="459"/>
+      <c r="G78" s="415"/>
+      <c r="H78" s="416"/>
+      <c r="I78" s="417"/>
+      <c r="J78" s="515"/>
+      <c r="K78" s="516"/>
+      <c r="L78" s="517"/>
+    </row>
+    <row r="79" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>62</v>
       </c>
@@ -7961,8 +7980,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:134" ht="15" customHeight="1">
-      <c r="A80" s="346" t="s">
+    <row r="80" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="344" t="s">
         <v>75</v>
       </c>
       <c r="B80" s="140" t="s">
@@ -7977,7 +7996,7 @@
       <c r="E80" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="F80" s="412" t="s">
+      <c r="F80" s="418" t="s">
         <v>50</v>
       </c>
       <c r="G80" s="90" t="s">
@@ -7986,17 +8005,17 @@
       <c r="H80" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="I80" s="441" t="s">
+      <c r="I80" s="446" t="s">
         <v>48</v>
       </c>
       <c r="J80" s="249" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="K80" s="250"/>
       <c r="L80" s="251"/>
     </row>
-    <row r="81" spans="1:134" ht="15" customHeight="1">
-      <c r="A81" s="347"/>
+    <row r="81" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="345"/>
       <c r="B81" s="141" t="s">
         <v>33</v>
       </c>
@@ -8009,24 +8028,24 @@
       <c r="E81" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="F81" s="413"/>
+      <c r="F81" s="419"/>
       <c r="G81" s="71" t="s">
         <v>116</v>
       </c>
       <c r="H81" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="I81" s="442"/>
+      <c r="I81" s="447"/>
       <c r="J81" s="165" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="K81" s="101"/>
       <c r="L81" s="166" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="82" spans="1:134" ht="15" customHeight="1">
-      <c r="A82" s="347"/>
+    <row r="82" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="345"/>
       <c r="B82" s="141" t="s">
         <v>47</v>
       </c>
@@ -8039,22 +8058,22 @@
       <c r="E82" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="F82" s="413"/>
+      <c r="F82" s="419"/>
       <c r="G82" s="278" t="s">
         <v>71</v>
       </c>
       <c r="H82" s="283" t="s">
-        <v>280</v>
-      </c>
-      <c r="I82" s="442"/>
-      <c r="J82" s="352" t="s">
-        <v>163</v>
-      </c>
-      <c r="K82" s="353"/>
+        <v>276</v>
+      </c>
+      <c r="I82" s="447"/>
+      <c r="J82" s="350" t="s">
+        <v>162</v>
+      </c>
+      <c r="K82" s="351"/>
       <c r="L82" s="297"/>
     </row>
-    <row r="83" spans="1:134" ht="15" customHeight="1">
-      <c r="A83" s="347"/>
+    <row r="83" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="345"/>
       <c r="B83" s="141" t="s">
         <v>43</v>
       </c>
@@ -8067,27 +8086,27 @@
       <c r="E83" s="163" t="s">
         <v>121</v>
       </c>
-      <c r="F83" s="413"/>
+      <c r="F83" s="419"/>
       <c r="G83" s="65" t="s">
         <v>120</v>
       </c>
       <c r="H83" s="82" t="s">
         <v>122</v>
       </c>
-      <c r="I83" s="442"/>
+      <c r="I83" s="447"/>
       <c r="J83" s="265" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K83" s="27"/>
       <c r="L83" s="41"/>
     </row>
-    <row r="84" spans="1:134" ht="15" customHeight="1">
-      <c r="A84" s="347"/>
+    <row r="84" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="345"/>
       <c r="B84" s="141" t="s">
         <v>41</v>
       </c>
       <c r="C84" s="160" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D84" s="40" t="s">
         <v>123</v>
@@ -8095,54 +8114,48 @@
       <c r="E84" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="F84" s="413"/>
+      <c r="F84" s="419"/>
       <c r="G84" s="71" t="s">
         <v>125</v>
       </c>
       <c r="H84" s="234" t="s">
-        <v>322</v>
-      </c>
-      <c r="I84" s="442"/>
+        <v>317</v>
+      </c>
+      <c r="I84" s="447"/>
       <c r="J84" s="266" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="K84" s="267" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L84" s="42"/>
     </row>
-    <row r="85" spans="1:134" ht="15" customHeight="1">
-      <c r="A85" s="347"/>
+    <row r="85" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="345"/>
       <c r="B85" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="C85" s="499" t="s">
-        <v>279</v>
-      </c>
-      <c r="D85" s="500"/>
+      <c r="C85" s="501" t="s">
+        <v>275</v>
+      </c>
+      <c r="D85" s="502"/>
       <c r="E85" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F85" s="413"/>
+      <c r="F85" s="419"/>
       <c r="G85" s="92" t="s">
-        <v>202</v>
-      </c>
-      <c r="H85" s="268" t="s">
-        <v>339</v>
-      </c>
-      <c r="I85" s="442"/>
+        <v>199</v>
+      </c>
+      <c r="H85" s="268"/>
+      <c r="I85" s="447"/>
       <c r="J85" s="266" t="s">
-        <v>248</v>
-      </c>
-      <c r="K85" s="268" t="s">
-        <v>341</v>
-      </c>
-      <c r="L85" s="273" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="86" spans="1:134" ht="15" customHeight="1">
-      <c r="A86" s="347"/>
+        <v>244</v>
+      </c>
+      <c r="K85" s="268"/>
+      <c r="L85" s="273"/>
+    </row>
+    <row r="86" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="345"/>
       <c r="B86" s="141" t="s">
         <v>35</v>
       </c>
@@ -8155,42 +8168,42 @@
       <c r="E86" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F86" s="413"/>
+      <c r="F86" s="419"/>
       <c r="G86" s="71" t="s">
         <v>133</v>
       </c>
       <c r="H86" s="42"/>
-      <c r="I86" s="442"/>
-      <c r="J86" s="360" t="s">
-        <v>275</v>
-      </c>
-      <c r="K86" s="294"/>
-      <c r="L86" s="295"/>
-    </row>
-    <row r="87" spans="1:134" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A87" s="347"/>
+      <c r="I86" s="447"/>
+      <c r="J86" s="358" t="s">
+        <v>271</v>
+      </c>
+      <c r="K86" s="359"/>
+      <c r="L86" s="360"/>
+    </row>
+    <row r="87" spans="1:134" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="345"/>
       <c r="B87" s="141" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C87" s="162" t="s">
         <v>118</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E87" s="40" t="s">
-        <v>263</v>
-      </c>
-      <c r="F87" s="413"/>
+        <v>259</v>
+      </c>
+      <c r="F87" s="419"/>
       <c r="G87" s="65" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H87" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="I87" s="442"/>
+        <v>257</v>
+      </c>
+      <c r="I87" s="447"/>
       <c r="J87" s="315" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K87" s="316"/>
       <c r="L87" s="330"/>
@@ -8317,8 +8330,8 @@
       <c r="EC87" s="30"/>
       <c r="ED87" s="30"/>
     </row>
-    <row r="88" spans="1:134" ht="15" customHeight="1">
-      <c r="A88" s="347"/>
+    <row r="88" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="345"/>
       <c r="B88" s="141" t="s">
         <v>31</v>
       </c>
@@ -8331,22 +8344,22 @@
       <c r="E88" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="F88" s="413"/>
+      <c r="F88" s="419"/>
       <c r="G88" s="75" t="s">
         <v>23</v>
       </c>
       <c r="H88" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="I88" s="442"/>
-      <c r="J88" s="529" t="s">
-        <v>266</v>
-      </c>
-      <c r="K88" s="530"/>
+      <c r="I88" s="447"/>
+      <c r="J88" s="531" t="s">
+        <v>262</v>
+      </c>
+      <c r="K88" s="532"/>
       <c r="L88" s="55"/>
     </row>
-    <row r="89" spans="1:134" ht="15" customHeight="1">
-      <c r="A89" s="347"/>
+    <row r="89" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="345"/>
       <c r="B89" s="141" t="s">
         <v>29</v>
       </c>
@@ -8357,50 +8370,50 @@
         <v>67</v>
       </c>
       <c r="E89" s="171" t="s">
-        <v>254</v>
-      </c>
-      <c r="F89" s="413"/>
+        <v>250</v>
+      </c>
+      <c r="F89" s="419"/>
       <c r="G89" s="75" t="s">
         <v>28</v>
       </c>
       <c r="H89" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="I89" s="442"/>
+        <v>210</v>
+      </c>
+      <c r="I89" s="447"/>
       <c r="J89" s="367" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="K89" s="368"/>
       <c r="L89" s="42"/>
     </row>
-    <row r="90" spans="1:134" ht="15" customHeight="1">
-      <c r="A90" s="347"/>
+    <row r="90" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="345"/>
       <c r="B90" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="C90" s="388" t="s">
-        <v>282</v>
-      </c>
-      <c r="D90" s="388"/>
-      <c r="E90" s="388"/>
-      <c r="F90" s="413"/>
+      <c r="C90" s="394" t="s">
+        <v>278</v>
+      </c>
+      <c r="D90" s="394"/>
+      <c r="E90" s="394"/>
+      <c r="F90" s="419"/>
       <c r="G90" s="93" t="s">
         <v>70</v>
       </c>
       <c r="H90" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="I90" s="442"/>
+        <v>236</v>
+      </c>
+      <c r="I90" s="447"/>
       <c r="J90" s="263" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K90" s="296" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="L90" s="297"/>
     </row>
-    <row r="91" spans="1:134" ht="15" customHeight="1">
-      <c r="A91" s="347"/>
+    <row r="91" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="345"/>
       <c r="B91" s="141" t="s">
         <v>24</v>
       </c>
@@ -8411,26 +8424,26 @@
         <v>26</v>
       </c>
       <c r="E91" s="269" t="s">
-        <v>344</v>
-      </c>
-      <c r="F91" s="413"/>
+        <v>331</v>
+      </c>
+      <c r="F91" s="419"/>
       <c r="G91" s="88" t="s">
         <v>150</v>
       </c>
       <c r="H91" s="213" t="s">
         <v>152</v>
       </c>
-      <c r="I91" s="442"/>
-      <c r="J91" s="387" t="s">
-        <v>274</v>
-      </c>
-      <c r="K91" s="388"/>
-      <c r="L91" s="389"/>
-    </row>
-    <row r="92" spans="1:134" ht="15" customHeight="1">
-      <c r="A92" s="347"/>
+      <c r="I91" s="447"/>
+      <c r="J91" s="393" t="s">
+        <v>270</v>
+      </c>
+      <c r="K91" s="394"/>
+      <c r="L91" s="395"/>
+    </row>
+    <row r="92" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="345"/>
       <c r="B92" s="142" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C92" s="139" t="s">
         <v>127</v>
@@ -8439,26 +8452,26 @@
         <v>128</v>
       </c>
       <c r="E92" s="176" t="s">
-        <v>218</v>
-      </c>
-      <c r="F92" s="413"/>
+        <v>215</v>
+      </c>
+      <c r="F92" s="419"/>
       <c r="G92" s="94" t="s">
         <v>153</v>
       </c>
       <c r="H92" s="191" t="s">
-        <v>295</v>
-      </c>
-      <c r="I92" s="442"/>
+        <v>291</v>
+      </c>
+      <c r="I92" s="447"/>
       <c r="J92" s="216" t="s">
         <v>34</v>
       </c>
       <c r="K92" s="270"/>
       <c r="L92" s="274"/>
     </row>
-    <row r="93" spans="1:134" ht="15" customHeight="1">
-      <c r="A93" s="347"/>
+    <row r="93" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="345"/>
       <c r="B93" s="142" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C93" s="132" t="s">
         <v>147</v>
@@ -8469,24 +8482,24 @@
       <c r="E93" s="171" t="s">
         <v>37</v>
       </c>
-      <c r="F93" s="413"/>
+      <c r="F93" s="419"/>
       <c r="G93" s="217" t="s">
         <v>151</v>
       </c>
       <c r="H93" s="66" t="s">
-        <v>262</v>
-      </c>
-      <c r="I93" s="442"/>
+        <v>258</v>
+      </c>
+      <c r="I93" s="447"/>
       <c r="J93" s="184" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K93" s="2"/>
       <c r="L93" s="42"/>
     </row>
-    <row r="94" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A94" s="347"/>
+    <row r="94" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="345"/>
       <c r="B94" s="143" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C94" s="39" t="s">
         <v>22</v>
@@ -8497,22 +8510,22 @@
       <c r="E94" s="174" t="s">
         <v>149</v>
       </c>
-      <c r="F94" s="413"/>
+      <c r="F94" s="419"/>
       <c r="G94" s="235" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="H94" s="157" t="s">
-        <v>229</v>
-      </c>
-      <c r="I94" s="454"/>
+        <v>225</v>
+      </c>
+      <c r="I94" s="459"/>
       <c r="J94" s="364" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="K94" s="365"/>
       <c r="L94" s="366"/>
     </row>
-    <row r="95" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A95" s="347"/>
+    <row r="95" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="345"/>
       <c r="B95" s="49" t="s">
         <v>19</v>
       </c>
@@ -8520,8 +8533,8 @@
         <v>18</v>
       </c>
       <c r="D95" s="309"/>
-      <c r="E95" s="445"/>
-      <c r="F95" s="413"/>
+      <c r="E95" s="450"/>
+      <c r="F95" s="419"/>
       <c r="G95" s="331" t="s">
         <v>65</v>
       </c>
@@ -8533,8 +8546,8 @@
       <c r="K95" s="309"/>
       <c r="L95" s="310"/>
     </row>
-    <row r="96" spans="1:134" ht="15" customHeight="1">
-      <c r="A96" s="347"/>
+    <row r="96" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="345"/>
       <c r="B96" s="155" t="s">
         <v>14</v>
       </c>
@@ -8543,33 +8556,33 @@
       </c>
       <c r="D96" s="304"/>
       <c r="E96" s="305"/>
-      <c r="F96" s="531"/>
-      <c r="G96" s="380" t="s">
+      <c r="F96" s="533"/>
+      <c r="G96" s="385" t="s">
+        <v>157</v>
+      </c>
+      <c r="H96" s="386"/>
+      <c r="I96" s="387"/>
+      <c r="J96" s="385" t="s">
         <v>158</v>
       </c>
-      <c r="H96" s="381"/>
-      <c r="I96" s="382"/>
-      <c r="J96" s="380" t="s">
-        <v>159</v>
-      </c>
-      <c r="K96" s="381"/>
-      <c r="L96" s="382"/>
-    </row>
-    <row r="97" spans="1:12" ht="15" customHeight="1">
-      <c r="A97" s="347"/>
+      <c r="K96" s="386"/>
+      <c r="L96" s="387"/>
+    </row>
+    <row r="97" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="345"/>
       <c r="B97" s="153" t="s">
         <v>12</v>
       </c>
       <c r="C97" s="95"/>
       <c r="D97" s="246" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E97" s="242" t="s">
         <v>32</v>
       </c>
-      <c r="F97" s="531"/>
+      <c r="F97" s="533"/>
       <c r="G97" s="317" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H97" s="318"/>
       <c r="I97" s="319"/>
@@ -8579,51 +8592,51 @@
       <c r="K97" s="312"/>
       <c r="L97" s="313"/>
     </row>
-    <row r="98" spans="1:12" ht="15" customHeight="1">
-      <c r="A98" s="347"/>
+    <row r="98" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="345"/>
       <c r="B98" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="533"/>
-      <c r="D98" s="534"/>
-      <c r="E98" s="535"/>
-      <c r="F98" s="531"/>
+      <c r="C98" s="535"/>
+      <c r="D98" s="536"/>
+      <c r="E98" s="537"/>
+      <c r="F98" s="533"/>
       <c r="G98" s="334"/>
       <c r="H98" s="335"/>
       <c r="I98" s="336"/>
       <c r="J98" s="306" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K98" s="307"/>
       <c r="L98" s="343"/>
     </row>
-    <row r="99" spans="1:12" ht="15" customHeight="1">
-      <c r="A99" s="347"/>
+    <row r="99" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="345"/>
       <c r="B99" s="153" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="370"/>
       <c r="D99" s="371"/>
       <c r="E99" s="372"/>
-      <c r="F99" s="531"/>
+      <c r="F99" s="533"/>
       <c r="G99" s="334"/>
       <c r="H99" s="335"/>
       <c r="I99" s="336"/>
       <c r="J99" s="306" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="K99" s="307"/>
       <c r="L99" s="343"/>
     </row>
-    <row r="100" spans="1:12" ht="15" customHeight="1">
-      <c r="A100" s="347"/>
+    <row r="100" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="345"/>
       <c r="B100" s="153" t="s">
         <v>6</v>
       </c>
       <c r="C100" s="370"/>
       <c r="D100" s="371"/>
       <c r="E100" s="372"/>
-      <c r="F100" s="531"/>
+      <c r="F100" s="533"/>
       <c r="G100" s="334"/>
       <c r="H100" s="335"/>
       <c r="I100" s="336"/>
@@ -8633,23 +8646,23 @@
       <c r="K100" s="323"/>
       <c r="L100" s="324"/>
     </row>
-    <row r="101" spans="1:12" ht="15" customHeight="1" thickBot="1">
-      <c r="A101" s="348"/>
+    <row r="101" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="346"/>
       <c r="B101" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="409"/>
-      <c r="D101" s="410"/>
-      <c r="E101" s="411"/>
-      <c r="F101" s="532"/>
-      <c r="G101" s="419"/>
-      <c r="H101" s="420"/>
-      <c r="I101" s="421"/>
-      <c r="J101" s="403"/>
-      <c r="K101" s="404"/>
-      <c r="L101" s="405"/>
-    </row>
-    <row r="102" spans="1:12" ht="15" customHeight="1" thickBot="1">
+      <c r="C101" s="415"/>
+      <c r="D101" s="416"/>
+      <c r="E101" s="417"/>
+      <c r="F101" s="534"/>
+      <c r="G101" s="425"/>
+      <c r="H101" s="426"/>
+      <c r="I101" s="427"/>
+      <c r="J101" s="409"/>
+      <c r="K101" s="410"/>
+      <c r="L101" s="411"/>
+    </row>
+    <row r="102" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>62</v>
       </c>
@@ -8669,10 +8682,10 @@
       <c r="G102" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H102" s="426" t="s">
+      <c r="H102" s="431" t="s">
         <v>58</v>
       </c>
-      <c r="I102" s="427"/>
+      <c r="I102" s="432"/>
       <c r="J102" s="14" t="s">
         <v>57</v>
       </c>
@@ -8683,8 +8696,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15" customHeight="1">
-      <c r="A103" s="346" t="s">
+    <row r="103" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="344" t="s">
         <v>54</v>
       </c>
       <c r="B103" s="140" t="s">
@@ -8697,26 +8710,26 @@
       <c r="E103" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F103" s="412" t="s">
+      <c r="F103" s="418" t="s">
         <v>50</v>
       </c>
       <c r="G103" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="H103" s="415" t="s">
-        <v>212</v>
-      </c>
-      <c r="I103" s="416"/>
+      <c r="H103" s="421" t="s">
+        <v>209</v>
+      </c>
+      <c r="I103" s="422"/>
       <c r="J103" s="287" t="s">
         <v>146</v>
       </c>
-      <c r="K103" s="519" t="s">
-        <v>337</v>
-      </c>
-      <c r="L103" s="520"/>
-    </row>
-    <row r="104" spans="1:12" ht="15" customHeight="1">
-      <c r="A104" s="347"/>
+      <c r="K103" s="521" t="s">
+        <v>327</v>
+      </c>
+      <c r="L103" s="522"/>
+    </row>
+    <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="345"/>
       <c r="B104" s="141" t="s">
         <v>47</v>
       </c>
@@ -8729,20 +8742,20 @@
       <c r="E104" s="205" t="s">
         <v>143</v>
       </c>
-      <c r="F104" s="413"/>
+      <c r="F104" s="419"/>
       <c r="G104" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="H104" s="417"/>
-      <c r="I104" s="418"/>
+      <c r="H104" s="423"/>
+      <c r="I104" s="424"/>
       <c r="J104" s="95"/>
       <c r="K104" s="238"/>
       <c r="L104" s="44"/>
     </row>
-    <row r="105" spans="1:12" ht="15" customHeight="1">
-      <c r="A105" s="347"/>
+    <row r="105" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="345"/>
       <c r="B105" s="141" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C105" s="204" t="s">
         <v>46</v>
@@ -8753,23 +8766,23 @@
       <c r="E105" s="202" t="s">
         <v>109</v>
       </c>
-      <c r="F105" s="413"/>
+      <c r="F105" s="419"/>
       <c r="G105" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="H105" s="417"/>
-      <c r="I105" s="418"/>
+      <c r="H105" s="423"/>
+      <c r="I105" s="424"/>
       <c r="J105" s="95"/>
       <c r="K105" s="238"/>
       <c r="L105" s="44"/>
     </row>
-    <row r="106" spans="1:12" ht="15" customHeight="1">
-      <c r="A106" s="347"/>
+    <row r="106" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="345"/>
       <c r="B106" s="141" t="s">
         <v>43</v>
       </c>
       <c r="C106" s="201" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D106" s="200" t="s">
         <v>142</v>
@@ -8777,18 +8790,18 @@
       <c r="E106" s="202" t="s">
         <v>42</v>
       </c>
-      <c r="F106" s="413"/>
+      <c r="F106" s="419"/>
       <c r="G106" s="178" t="s">
-        <v>236</v>
-      </c>
-      <c r="H106" s="417"/>
-      <c r="I106" s="418"/>
+        <v>232</v>
+      </c>
+      <c r="H106" s="423"/>
+      <c r="I106" s="424"/>
       <c r="J106" s="95"/>
       <c r="K106" s="238"/>
       <c r="L106" s="44"/>
     </row>
-    <row r="107" spans="1:12" ht="15" customHeight="1">
-      <c r="A107" s="347"/>
+    <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="345"/>
       <c r="B107" s="141" t="s">
         <v>41</v>
       </c>
@@ -8799,20 +8812,20 @@
       <c r="E107" s="205" t="s">
         <v>88</v>
       </c>
-      <c r="F107" s="413"/>
+      <c r="F107" s="419"/>
       <c r="G107" s="170" t="s">
-        <v>227</v>
-      </c>
-      <c r="H107" s="417"/>
-      <c r="I107" s="418"/>
-      <c r="J107" s="360" t="s">
-        <v>275</v>
-      </c>
-      <c r="K107" s="294"/>
-      <c r="L107" s="295"/>
-    </row>
-    <row r="108" spans="1:12" ht="15" customHeight="1">
-      <c r="A108" s="347"/>
+        <v>223</v>
+      </c>
+      <c r="H107" s="423"/>
+      <c r="I107" s="424"/>
+      <c r="J107" s="358" t="s">
+        <v>271</v>
+      </c>
+      <c r="K107" s="359"/>
+      <c r="L107" s="360"/>
+    </row>
+    <row r="108" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="345"/>
       <c r="B108" s="141" t="s">
         <v>38</v>
       </c>
@@ -8825,18 +8838,18 @@
       <c r="E108" s="202" t="s">
         <v>69</v>
       </c>
-      <c r="F108" s="413"/>
+      <c r="F108" s="419"/>
       <c r="G108" s="167" t="s">
         <v>36</v>
       </c>
-      <c r="H108" s="417"/>
-      <c r="I108" s="418"/>
+      <c r="H108" s="423"/>
+      <c r="I108" s="424"/>
       <c r="J108" s="99"/>
       <c r="K108" s="290"/>
       <c r="L108" s="44"/>
     </row>
-    <row r="109" spans="1:12" ht="15" customHeight="1">
-      <c r="A109" s="347"/>
+    <row r="109" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="345"/>
       <c r="B109" s="141" t="s">
         <v>35</v>
       </c>
@@ -8849,20 +8862,20 @@
       <c r="E109" s="195" t="s">
         <v>37</v>
       </c>
-      <c r="F109" s="413"/>
+      <c r="F109" s="419"/>
       <c r="G109" s="225" t="s">
-        <v>324</v>
-      </c>
-      <c r="H109" s="417"/>
-      <c r="I109" s="418"/>
-      <c r="J109" s="360" t="s">
-        <v>164</v>
-      </c>
-      <c r="K109" s="294"/>
-      <c r="L109" s="295"/>
-    </row>
-    <row r="110" spans="1:12" ht="15" customHeight="1">
-      <c r="A110" s="347"/>
+        <v>319</v>
+      </c>
+      <c r="H109" s="423"/>
+      <c r="I109" s="424"/>
+      <c r="J109" s="358" t="s">
+        <v>163</v>
+      </c>
+      <c r="K109" s="359"/>
+      <c r="L109" s="360"/>
+    </row>
+    <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="345"/>
       <c r="B110" s="141" t="s">
         <v>33</v>
       </c>
@@ -8875,44 +8888,44 @@
       <c r="E110" s="195" t="s">
         <v>149</v>
       </c>
-      <c r="F110" s="413"/>
+      <c r="F110" s="419"/>
       <c r="G110" s="164" t="s">
-        <v>165</v>
-      </c>
-      <c r="H110" s="417"/>
-      <c r="I110" s="418"/>
+        <v>164</v>
+      </c>
+      <c r="H110" s="423"/>
+      <c r="I110" s="424"/>
       <c r="J110" s="289" t="s">
         <v>100</v>
       </c>
       <c r="K110" s="238"/>
       <c r="L110" s="44"/>
     </row>
-    <row r="111" spans="1:12" ht="15" customHeight="1">
-      <c r="A111" s="347"/>
+    <row r="111" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="345"/>
       <c r="B111" s="141" t="s">
         <v>31</v>
       </c>
       <c r="C111" s="203" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="62" t="s">
-        <v>217</v>
-      </c>
-      <c r="F111" s="413"/>
+        <v>214</v>
+      </c>
+      <c r="F111" s="419"/>
       <c r="G111" s="164" t="s">
         <v>150</v>
       </c>
-      <c r="H111" s="417"/>
-      <c r="I111" s="418"/>
+      <c r="H111" s="423"/>
+      <c r="I111" s="424"/>
       <c r="J111" s="288" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="K111" s="28"/>
       <c r="L111" s="45"/>
     </row>
-    <row r="112" spans="1:12" ht="15" customHeight="1">
-      <c r="A112" s="347"/>
+    <row r="112" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="345"/>
       <c r="B112" s="141" t="s">
         <v>29</v>
       </c>
@@ -8921,20 +8934,20 @@
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="63" t="s">
-        <v>312</v>
-      </c>
-      <c r="F112" s="413"/>
+        <v>307</v>
+      </c>
+      <c r="F112" s="419"/>
       <c r="G112" s="190"/>
-      <c r="H112" s="417"/>
-      <c r="I112" s="418"/>
-      <c r="J112" s="387" t="s">
-        <v>299</v>
-      </c>
-      <c r="K112" s="388"/>
-      <c r="L112" s="389"/>
-    </row>
-    <row r="113" spans="1:134" ht="15" customHeight="1">
-      <c r="A113" s="347"/>
+      <c r="H112" s="423"/>
+      <c r="I112" s="424"/>
+      <c r="J112" s="393" t="s">
+        <v>294</v>
+      </c>
+      <c r="K112" s="394"/>
+      <c r="L112" s="395"/>
+    </row>
+    <row r="113" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="345"/>
       <c r="B113" s="141" t="s">
         <v>25</v>
       </c>
@@ -8947,17 +8960,17 @@
       <c r="E113" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="F113" s="413"/>
-      <c r="H113" s="417"/>
-      <c r="I113" s="418"/>
+      <c r="F113" s="419"/>
+      <c r="H113" s="423"/>
+      <c r="I113" s="424"/>
       <c r="J113" s="281"/>
-      <c r="K113" s="422" t="s">
-        <v>265</v>
-      </c>
-      <c r="L113" s="423"/>
-    </row>
-    <row r="114" spans="1:134" ht="15" customHeight="1">
-      <c r="A114" s="347"/>
+      <c r="K113" s="428" t="s">
+        <v>261</v>
+      </c>
+      <c r="L113" s="381"/>
+    </row>
+    <row r="114" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="345"/>
       <c r="B114" s="141" t="s">
         <v>24</v>
       </c>
@@ -8965,85 +8978,85 @@
         <v>153</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="E114" s="537" t="s">
-        <v>305</v>
-      </c>
-      <c r="F114" s="413"/>
+        <v>207</v>
+      </c>
+      <c r="E114" s="295" t="s">
+        <v>300</v>
+      </c>
+      <c r="F114" s="419"/>
       <c r="G114" s="237"/>
-      <c r="H114" s="417"/>
-      <c r="I114" s="418"/>
+      <c r="H114" s="423"/>
+      <c r="I114" s="424"/>
       <c r="J114" s="99"/>
       <c r="K114" s="238"/>
       <c r="L114" s="44"/>
     </row>
-    <row r="115" spans="1:134" ht="15" customHeight="1">
-      <c r="A115" s="347"/>
+    <row r="115" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="345"/>
       <c r="B115" s="146" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C115" s="95"/>
       <c r="D115" s="194" t="s">
         <v>154</v>
       </c>
-      <c r="E115" s="536" t="s">
-        <v>345</v>
-      </c>
-      <c r="F115" s="413"/>
+      <c r="E115" s="294" t="s">
+        <v>332</v>
+      </c>
+      <c r="F115" s="419"/>
       <c r="G115" s="179"/>
-      <c r="H115" s="417"/>
-      <c r="I115" s="418"/>
+      <c r="H115" s="423"/>
+      <c r="I115" s="424"/>
       <c r="J115" s="136" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="K115" s="13"/>
       <c r="L115" s="46"/>
     </row>
-    <row r="116" spans="1:134" ht="15" customHeight="1">
-      <c r="A116" s="347"/>
+    <row r="116" spans="1:134" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="345"/>
       <c r="B116" s="146" t="s">
-        <v>242</v>
-      </c>
-      <c r="C116" s="394" t="s">
-        <v>310</v>
-      </c>
-      <c r="D116" s="395"/>
-      <c r="E116" s="396"/>
-      <c r="F116" s="413"/>
+        <v>238</v>
+      </c>
+      <c r="C116" s="400" t="s">
+        <v>305</v>
+      </c>
+      <c r="D116" s="401"/>
+      <c r="E116" s="402"/>
+      <c r="F116" s="419"/>
       <c r="G116" s="206" t="s">
-        <v>311</v>
-      </c>
-      <c r="H116" s="417"/>
-      <c r="I116" s="418"/>
+        <v>306</v>
+      </c>
+      <c r="H116" s="423"/>
+      <c r="I116" s="424"/>
       <c r="J116" s="306" t="s">
-        <v>320</v>
-      </c>
-      <c r="K116" s="390"/>
+        <v>315</v>
+      </c>
+      <c r="K116" s="396"/>
       <c r="L116" s="215"/>
     </row>
-    <row r="117" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="347"/>
+    <row r="117" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="345"/>
       <c r="B117" s="147" t="s">
-        <v>243</v>
-      </c>
-      <c r="C117" s="501" t="s">
-        <v>268</v>
-      </c>
-      <c r="D117" s="502"/>
-      <c r="E117" s="503"/>
-      <c r="F117" s="414"/>
+        <v>239</v>
+      </c>
+      <c r="C117" s="503" t="s">
+        <v>264</v>
+      </c>
+      <c r="D117" s="504"/>
+      <c r="E117" s="505"/>
+      <c r="F117" s="420"/>
       <c r="G117" s="182"/>
-      <c r="H117" s="417"/>
-      <c r="I117" s="418"/>
+      <c r="H117" s="423"/>
+      <c r="I117" s="424"/>
       <c r="J117" s="362" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K117" s="363"/>
       <c r="L117" s="47"/>
     </row>
-    <row r="118" spans="1:134" ht="15" customHeight="1" thickBot="1">
-      <c r="A118" s="347"/>
+    <row r="118" spans="1:134" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="345"/>
       <c r="B118" s="150" t="s">
         <v>19</v>
       </c>
@@ -9064,8 +9077,8 @@
       <c r="K118" s="309"/>
       <c r="L118" s="310"/>
     </row>
-    <row r="119" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A119" s="347"/>
+    <row r="119" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="345"/>
       <c r="B119" s="155" t="s">
         <v>12</v>
       </c>
@@ -9074,19 +9087,19 @@
       </c>
       <c r="D119" s="374"/>
       <c r="E119" s="375"/>
-      <c r="F119" s="349" t="s">
+      <c r="F119" s="347" t="s">
         <v>50</v>
       </c>
-      <c r="G119" s="492" t="s">
+      <c r="G119" s="494" t="s">
         <v>13</v>
       </c>
-      <c r="H119" s="474"/>
-      <c r="I119" s="493"/>
-      <c r="J119" s="492" t="s">
+      <c r="H119" s="476"/>
+      <c r="I119" s="495"/>
+      <c r="J119" s="494" t="s">
         <v>83</v>
       </c>
-      <c r="K119" s="474"/>
-      <c r="L119" s="475"/>
+      <c r="K119" s="476"/>
+      <c r="L119" s="477"/>
       <c r="M119" s="7"/>
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
@@ -9210,22 +9223,22 @@
       <c r="EC119" s="7"/>
       <c r="ED119" s="7"/>
     </row>
-    <row r="120" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A120" s="347"/>
+    <row r="120" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="345"/>
       <c r="B120" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="357" t="s">
-        <v>287</v>
-      </c>
-      <c r="D120" s="358"/>
-      <c r="E120" s="359"/>
-      <c r="F120" s="350"/>
-      <c r="G120" s="470" t="s">
+      <c r="C120" s="355" t="s">
+        <v>283</v>
+      </c>
+      <c r="D120" s="356"/>
+      <c r="E120" s="357"/>
+      <c r="F120" s="348"/>
+      <c r="G120" s="469" t="s">
         <v>155</v>
       </c>
-      <c r="H120" s="471"/>
-      <c r="I120" s="471"/>
+      <c r="H120" s="470"/>
+      <c r="I120" s="470"/>
       <c r="J120" s="311" t="s">
         <v>10</v>
       </c>
@@ -9354,19 +9367,19 @@
       <c r="EC120" s="7"/>
       <c r="ED120" s="7"/>
     </row>
-    <row r="121" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A121" s="347"/>
+    <row r="121" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="345"/>
       <c r="B121" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="C121" s="394" t="s">
+      <c r="C121" s="400" t="s">
         <v>138</v>
       </c>
-      <c r="D121" s="395"/>
-      <c r="E121" s="396"/>
-      <c r="F121" s="350"/>
+      <c r="D121" s="401"/>
+      <c r="E121" s="402"/>
+      <c r="F121" s="348"/>
       <c r="G121" s="306" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="H121" s="307"/>
       <c r="I121" s="307"/>
@@ -9496,25 +9509,25 @@
       <c r="EC121" s="7"/>
       <c r="ED121" s="7"/>
     </row>
-    <row r="122" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A122" s="347"/>
+    <row r="122" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="345"/>
       <c r="B122" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="C122" s="394" t="s">
+      <c r="C122" s="400" t="s">
         <v>139</v>
       </c>
-      <c r="D122" s="395"/>
-      <c r="E122" s="396"/>
-      <c r="F122" s="350"/>
+      <c r="D122" s="401"/>
+      <c r="E122" s="402"/>
+      <c r="F122" s="348"/>
       <c r="G122" s="376"/>
       <c r="H122" s="377"/>
       <c r="I122" s="377"/>
-      <c r="J122" s="387" t="s">
-        <v>192</v>
-      </c>
-      <c r="K122" s="388"/>
-      <c r="L122" s="389"/>
+      <c r="J122" s="393" t="s">
+        <v>189</v>
+      </c>
+      <c r="K122" s="394"/>
+      <c r="L122" s="395"/>
       <c r="M122" s="7"/>
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
@@ -9638,27 +9651,27 @@
       <c r="EC122" s="7"/>
       <c r="ED122" s="7"/>
     </row>
-    <row r="123" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A123" s="347"/>
+    <row r="123" spans="1:134" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="345"/>
       <c r="B123" s="153" t="s">
         <v>6</v>
       </c>
-      <c r="C123" s="357" t="s">
-        <v>296</v>
-      </c>
-      <c r="D123" s="358"/>
-      <c r="E123" s="359"/>
-      <c r="F123" s="350"/>
-      <c r="G123" s="354" t="s">
-        <v>309</v>
-      </c>
-      <c r="H123" s="355"/>
-      <c r="I123" s="356"/>
-      <c r="J123" s="431" t="s">
-        <v>307</v>
-      </c>
-      <c r="K123" s="432"/>
-      <c r="L123" s="433"/>
+      <c r="C123" s="355" t="s">
+        <v>292</v>
+      </c>
+      <c r="D123" s="356"/>
+      <c r="E123" s="357"/>
+      <c r="F123" s="348"/>
+      <c r="G123" s="352" t="s">
+        <v>304</v>
+      </c>
+      <c r="H123" s="353"/>
+      <c r="I123" s="354"/>
+      <c r="J123" s="436" t="s">
+        <v>302</v>
+      </c>
+      <c r="K123" s="437"/>
+      <c r="L123" s="438"/>
       <c r="M123" s="7"/>
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
@@ -9782,29 +9795,29 @@
       <c r="EC123" s="7"/>
       <c r="ED123" s="7"/>
     </row>
-    <row r="124" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A124" s="348"/>
+    <row r="124" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="346"/>
       <c r="B124" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="C124" s="424" t="s">
-        <v>179</v>
-      </c>
-      <c r="D124" s="424"/>
-      <c r="E124" s="425"/>
-      <c r="F124" s="351"/>
-      <c r="G124" s="494" t="s">
-        <v>306</v>
-      </c>
-      <c r="H124" s="495"/>
-      <c r="I124" s="495"/>
-      <c r="J124" s="428" t="s">
-        <v>308</v>
-      </c>
-      <c r="K124" s="429"/>
-      <c r="L124" s="430"/>
-    </row>
-    <row r="125" spans="1:134" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="C124" s="429" t="s">
+        <v>176</v>
+      </c>
+      <c r="D124" s="429"/>
+      <c r="E124" s="430"/>
+      <c r="F124" s="349"/>
+      <c r="G124" s="496" t="s">
+        <v>301</v>
+      </c>
+      <c r="H124" s="497"/>
+      <c r="I124" s="497"/>
+      <c r="J124" s="433" t="s">
+        <v>303</v>
+      </c>
+      <c r="K124" s="434"/>
+      <c r="L124" s="435"/>
+    </row>
+    <row r="125" spans="1:134" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="209"/>
       <c r="F125" s="210"/>
       <c r="M125" s="7"/>
@@ -9888,29 +9901,29 @@
       <c r="CM125" s="7"/>
       <c r="CN125" s="7"/>
     </row>
-    <row r="126" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B126" s="402"/>
-      <c r="C126" s="408" t="s">
-        <v>267</v>
-      </c>
-      <c r="D126" s="408"/>
-      <c r="E126" s="408"/>
-    </row>
-    <row r="127" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B127" s="402"/>
-      <c r="C127" s="408" t="s">
-        <v>269</v>
-      </c>
-      <c r="D127" s="408"/>
-      <c r="E127" s="408"/>
+    <row r="126" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="408"/>
+      <c r="C126" s="414" t="s">
+        <v>263</v>
+      </c>
+      <c r="D126" s="414"/>
+      <c r="E126" s="414"/>
+    </row>
+    <row r="127" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="408"/>
+      <c r="C127" s="414" t="s">
+        <v>265</v>
+      </c>
+      <c r="D127" s="414"/>
+      <c r="E127" s="414"/>
       <c r="G127" s="36"/>
       <c r="H127" s="34"/>
       <c r="K127" s="34"/>
-      <c r="L127" s="407"/>
-      <c r="M127" s="407"/>
-    </row>
-    <row r="128" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B128" s="402"/>
+      <c r="L127" s="413"/>
+      <c r="M127" s="413"/>
+    </row>
+    <row r="128" spans="1:134" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="408"/>
       <c r="C128" s="59"/>
       <c r="D128" s="59"/>
       <c r="E128" s="59"/>
@@ -9921,37 +9934,37 @@
       </c>
       <c r="M128" s="18"/>
     </row>
-    <row r="129" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B129" s="402"/>
+    <row r="129" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B129" s="408"/>
       <c r="C129" s="58"/>
       <c r="D129" s="58"/>
       <c r="E129" s="58"/>
       <c r="G129" s="36"/>
       <c r="H129" s="36"/>
-      <c r="K129" s="406"/>
-      <c r="L129" s="406"/>
-      <c r="M129" s="406"/>
-    </row>
-    <row r="130" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B130" s="402"/>
+      <c r="K129" s="412"/>
+      <c r="L129" s="412"/>
+      <c r="M129" s="412"/>
+    </row>
+    <row r="130" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B130" s="408"/>
       <c r="D130" s="58"/>
       <c r="E130" s="58"/>
       <c r="G130" s="36"/>
       <c r="H130" s="36"/>
       <c r="K130" s="18"/>
-      <c r="L130" s="408"/>
-      <c r="M130" s="408"/>
-    </row>
-    <row r="131" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B131" s="402"/>
+      <c r="L130" s="414"/>
+      <c r="M130" s="414"/>
+    </row>
+    <row r="131" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="408"/>
       <c r="G131" s="34"/>
       <c r="H131" s="34"/>
-      <c r="K131" s="406"/>
-      <c r="L131" s="406"/>
+      <c r="K131" s="412"/>
+      <c r="L131" s="412"/>
       <c r="M131" s="34"/>
     </row>
-    <row r="132" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B132" s="402"/>
+    <row r="132" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="408"/>
       <c r="C132" s="58"/>
       <c r="D132" s="59"/>
       <c r="E132" s="58"/>
@@ -9959,48 +9972,48 @@
       <c r="H132" s="34"/>
       <c r="K132" s="34"/>
     </row>
-    <row r="133" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B133" s="402"/>
+    <row r="133" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B133" s="408"/>
       <c r="C133" s="59"/>
       <c r="D133" s="59"/>
       <c r="E133" s="20"/>
-      <c r="G133" s="406"/>
-      <c r="H133" s="406"/>
-      <c r="K133" s="406"/>
-      <c r="L133" s="406"/>
+      <c r="G133" s="412"/>
+      <c r="H133" s="412"/>
+      <c r="K133" s="412"/>
+      <c r="L133" s="412"/>
       <c r="M133" s="34"/>
     </row>
-    <row r="134" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B134" s="402"/>
-      <c r="C134" s="491"/>
-      <c r="D134" s="491"/>
-      <c r="E134" s="491"/>
+    <row r="134" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B134" s="408"/>
+      <c r="C134" s="493"/>
+      <c r="D134" s="493"/>
+      <c r="E134" s="493"/>
       <c r="G134" s="34"/>
       <c r="H134" s="19"/>
-      <c r="K134" s="406"/>
-      <c r="L134" s="406"/>
-      <c r="M134" s="406"/>
-    </row>
-    <row r="135" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B135" s="402"/>
+      <c r="K134" s="412"/>
+      <c r="L134" s="412"/>
+      <c r="M134" s="412"/>
+    </row>
+    <row r="135" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B135" s="408"/>
       <c r="C135" s="59"/>
-      <c r="D135" s="406"/>
-      <c r="E135" s="406"/>
-      <c r="K135" s="491"/>
-      <c r="L135" s="491"/>
-      <c r="M135" s="491"/>
-    </row>
-    <row r="136" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B136" s="402"/>
+      <c r="D135" s="412"/>
+      <c r="E135" s="412"/>
+      <c r="K135" s="493"/>
+      <c r="L135" s="493"/>
+      <c r="M135" s="493"/>
+    </row>
+    <row r="136" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="408"/>
       <c r="C136" s="58"/>
       <c r="D136" s="58"/>
       <c r="E136" s="58"/>
-      <c r="K136" s="406"/>
-      <c r="L136" s="406"/>
-      <c r="M136" s="406"/>
-    </row>
-    <row r="137" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B137" s="402"/>
+      <c r="K136" s="412"/>
+      <c r="L136" s="412"/>
+      <c r="M136" s="412"/>
+    </row>
+    <row r="137" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="408"/>
       <c r="C137" s="58"/>
       <c r="D137" s="58"/>
       <c r="E137" s="58"/>
@@ -10008,106 +10021,104 @@
       <c r="L137" s="34"/>
       <c r="M137" s="34"/>
     </row>
-    <row r="138" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B138" s="402"/>
+    <row r="138" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B138" s="408"/>
       <c r="D138" s="58"/>
-      <c r="G138" s="406"/>
-      <c r="H138" s="406"/>
+      <c r="G138" s="412"/>
+      <c r="H138" s="412"/>
       <c r="I138" s="21"/>
-      <c r="L138" s="406"/>
-      <c r="M138" s="406"/>
-    </row>
-    <row r="139" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B139" s="402"/>
+      <c r="L138" s="412"/>
+      <c r="M138" s="412"/>
+    </row>
+    <row r="139" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B139" s="408"/>
       <c r="G139" s="34"/>
       <c r="H139" s="34"/>
       <c r="I139" s="21"/>
-      <c r="K139" s="406"/>
-      <c r="L139" s="406"/>
-      <c r="M139" s="406"/>
-    </row>
-    <row r="140" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="K139" s="412"/>
+      <c r="L139" s="412"/>
+      <c r="M139" s="412"/>
+    </row>
+    <row r="140" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G140" s="34"/>
-      <c r="H140" s="406"/>
-      <c r="I140" s="406"/>
-      <c r="K140" s="408"/>
-      <c r="L140" s="408"/>
-      <c r="M140" s="408"/>
-    </row>
-    <row r="141" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="G141" s="408"/>
-      <c r="H141" s="408"/>
-      <c r="I141" s="408"/>
-    </row>
-    <row r="142" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="G142" s="406"/>
-      <c r="H142" s="406"/>
-    </row>
-    <row r="143" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="144" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="G144" s="406"/>
-      <c r="H144" s="406"/>
-    </row>
-    <row r="145" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="146" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="147" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="148" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="149" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="H140" s="412"/>
+      <c r="I140" s="412"/>
+      <c r="K140" s="414"/>
+      <c r="L140" s="414"/>
+      <c r="M140" s="414"/>
+    </row>
+    <row r="141" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G141" s="414"/>
+      <c r="H141" s="414"/>
+      <c r="I141" s="414"/>
+    </row>
+    <row r="142" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G142" s="412"/>
+      <c r="H142" s="412"/>
+    </row>
+    <row r="143" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" spans="2:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G144" s="412"/>
+      <c r="H144" s="412"/>
+    </row>
+    <row r="145" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E149" s="36"/>
       <c r="F149" s="34"/>
     </row>
-    <row r="150" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="E150" s="406"/>
-      <c r="F150" s="406"/>
-    </row>
-    <row r="151" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="150" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E150" s="412"/>
+      <c r="F150" s="412"/>
+    </row>
+    <row r="151" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E151" s="34"/>
       <c r="F151" s="34"/>
     </row>
-    <row r="152" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="152" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E152" s="36"/>
       <c r="F152" s="36"/>
     </row>
-    <row r="153" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="153" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E153" s="36"/>
       <c r="F153" s="34"/>
     </row>
-    <row r="154" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="154" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E154" s="36"/>
     </row>
-    <row r="155" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="155" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E155" s="34"/>
       <c r="F155" s="34"/>
     </row>
-    <row r="156" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="156" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E156" s="34"/>
       <c r="F156" s="34"/>
     </row>
-    <row r="157" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="157" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E157" s="34"/>
       <c r="F157" s="34"/>
     </row>
-    <row r="158" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="158" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E158" s="34"/>
       <c r="F158" s="36"/>
     </row>
-    <row r="159" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="159" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E159" s="36"/>
       <c r="F159" s="36"/>
     </row>
-    <row r="160" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="160" spans="5:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E160" s="20"/>
       <c r="F160" s="34"/>
     </row>
-    <row r="161" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="162" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="163" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="164" s="7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="165" s="7" customFormat="1" ht="15" customHeight="1"/>
+    <row r="161" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="209">
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C74:E74"/>
     <mergeCell ref="G77:I77"/>
     <mergeCell ref="J95:L95"/>
     <mergeCell ref="C53:E53"/>
@@ -10129,7 +10140,7 @@
     <mergeCell ref="F31:F54"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C98:E98"/>
-    <mergeCell ref="G124:I124"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C116:E116"/>
@@ -10153,7 +10164,7 @@
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="K103:L103"/>
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
     <mergeCell ref="E150:F150"/>
     <mergeCell ref="C134:E134"/>
     <mergeCell ref="D135:E135"/>
@@ -10177,15 +10188,7 @@
     <mergeCell ref="C122:E122"/>
     <mergeCell ref="K131:L131"/>
     <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="I31:I45"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="G124:I124"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="J26:K26"/>
@@ -10195,6 +10198,16 @@
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="J24:L24"/>
     <mergeCell ref="J39:K39"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="I31:I45"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="K36:L36"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="G100:I100"/>
@@ -10291,7 +10304,6 @@
     <mergeCell ref="C73:E73"/>
     <mergeCell ref="G73:I73"/>
     <mergeCell ref="G72:I72"/>
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="C118:E118"/>
     <mergeCell ref="G67:H67"/>
@@ -10312,9 +10324,10 @@
     <mergeCell ref="J29:L29"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="G48:I48"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C74:E74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>

</xml_diff>